<commit_message>
App skeleton with all dependencies
</commit_message>
<xml_diff>
--- a/documentos/plantilla ABP.xlsx
+++ b/documentos/plantilla ABP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="SDM" sheetId="13" r:id="rId11"/>
     <sheet name="SMA" sheetId="14" r:id="rId12"/>
     <sheet name="NM" sheetId="15" r:id="rId13"/>
+    <sheet name="PD1" sheetId="17" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="Graficos1">TAG!$F$8:$H$21</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="420">
   <si>
     <t>Apellidos</t>
   </si>
@@ -3036,7 +3037,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3298,6 +3299,15 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3655,7 +3665,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="64">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4626,113 +4648,113 @@
   <sheetData>
     <row r="1" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="171" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="163"/>
-      <c r="N2" s="163"/>
-      <c r="O2" s="163"/>
-      <c r="P2" s="163"/>
-      <c r="Q2" s="163"/>
-      <c r="R2" s="164"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="172"/>
+      <c r="O2" s="172"/>
+      <c r="P2" s="172"/>
+      <c r="Q2" s="172"/>
+      <c r="R2" s="173"/>
     </row>
     <row r="3" spans="2:18" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="174" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
-      <c r="F3" s="166"/>
-      <c r="G3" s="166"/>
-      <c r="H3" s="166"/>
-      <c r="I3" s="166"/>
-      <c r="J3" s="166"/>
-      <c r="K3" s="166"/>
-      <c r="L3" s="166"/>
-      <c r="M3" s="166"/>
-      <c r="N3" s="166"/>
-      <c r="O3" s="166"/>
-      <c r="P3" s="166"/>
-      <c r="Q3" s="166"/>
-      <c r="R3" s="167"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
+      <c r="J3" s="175"/>
+      <c r="K3" s="175"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
+      <c r="O3" s="175"/>
+      <c r="P3" s="175"/>
+      <c r="Q3" s="175"/>
+      <c r="R3" s="176"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="180" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
-      <c r="H4" s="172"/>
-      <c r="I4" s="172"/>
-      <c r="J4" s="172"/>
-      <c r="K4" s="172"/>
-      <c r="L4" s="172"/>
-      <c r="M4" s="172"/>
-      <c r="N4" s="172"/>
-      <c r="O4" s="172"/>
-      <c r="P4" s="172"/>
-      <c r="Q4" s="172"/>
-      <c r="R4" s="173"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="181"/>
+      <c r="K4" s="181"/>
+      <c r="L4" s="181"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="181"/>
+      <c r="O4" s="181"/>
+      <c r="P4" s="181"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="182"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="174" t="s">
+      <c r="B5" s="183" t="s">
         <v>271</v>
       </c>
-      <c r="C5" s="175" t="s">
+      <c r="C5" s="184" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="175"/>
-      <c r="E5" s="175"/>
-      <c r="F5" s="175"/>
-      <c r="G5" s="175"/>
-      <c r="H5" s="175"/>
-      <c r="I5" s="175"/>
-      <c r="J5" s="175"/>
-      <c r="K5" s="175"/>
-      <c r="L5" s="175"/>
-      <c r="M5" s="175"/>
-      <c r="N5" s="175"/>
-      <c r="O5" s="175"/>
-      <c r="P5" s="175"/>
-      <c r="Q5" s="175"/>
-      <c r="R5" s="176"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="184"/>
+      <c r="H5" s="184"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
+      <c r="K5" s="184"/>
+      <c r="L5" s="184"/>
+      <c r="M5" s="184"/>
+      <c r="N5" s="184"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="184"/>
+      <c r="Q5" s="184"/>
+      <c r="R5" s="185"/>
     </row>
     <row r="6" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="168" t="s">
+      <c r="B6" s="177" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="169" t="s">
+      <c r="C6" s="178" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="169"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="169"/>
-      <c r="H6" s="169"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="169"/>
-      <c r="K6" s="169"/>
-      <c r="L6" s="169"/>
-      <c r="M6" s="169"/>
-      <c r="N6" s="169"/>
-      <c r="O6" s="169"/>
-      <c r="P6" s="169"/>
-      <c r="Q6" s="169"/>
-      <c r="R6" s="170"/>
+      <c r="D6" s="178"/>
+      <c r="E6" s="178"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="178"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="178"/>
+      <c r="J6" s="178"/>
+      <c r="K6" s="178"/>
+      <c r="L6" s="178"/>
+      <c r="M6" s="178"/>
+      <c r="N6" s="178"/>
+      <c r="O6" s="178"/>
+      <c r="P6" s="178"/>
+      <c r="Q6" s="178"/>
+      <c r="R6" s="179"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="47"/>
@@ -4776,32 +4798,32 @@
       <c r="B9" s="90" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="177" t="s">
+      <c r="C9" s="186" t="s">
         <v>417</v>
       </c>
-      <c r="D9" s="177"/>
-      <c r="E9" s="177"/>
-      <c r="F9" s="178"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="186"/>
+      <c r="F9" s="187"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E11" s="159" t="s">
+      <c r="E11" s="168" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="159"/>
-      <c r="G11" s="160" t="s">
+      <c r="F11" s="168"/>
+      <c r="G11" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="160"/>
-      <c r="K11" s="160"/>
-      <c r="L11" s="161" t="s">
+      <c r="H11" s="169"/>
+      <c r="I11" s="169"/>
+      <c r="J11" s="169"/>
+      <c r="K11" s="169"/>
+      <c r="L11" s="170" t="s">
         <v>6</v>
       </c>
-      <c r="M11" s="161"/>
-      <c r="N11" s="161"/>
-      <c r="O11" s="161"/>
-      <c r="P11" s="161"/>
+      <c r="M11" s="170"/>
+      <c r="N11" s="170"/>
+      <c r="O11" s="170"/>
+      <c r="P11" s="170"/>
     </row>
     <row r="12" spans="2:18" s="53" customFormat="1" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="48" t="s">
@@ -5195,32 +5217,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>364</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="223" t="s">
+      <c r="B3" s="232" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="225"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -5313,32 +5335,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>367</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="223" t="s">
+      <c r="B3" s="232" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="225"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -5444,93 +5466,93 @@
       <c r="P1" s="12"/>
     </row>
     <row r="2" spans="2:16" ht="23.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>405</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="192"/>
       <c r="M2" s="86"/>
       <c r="N2" s="86"/>
       <c r="O2" s="86"/>
       <c r="P2" s="12"/>
     </row>
     <row r="3" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>407</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="195"/>
       <c r="M3" s="125"/>
       <c r="N3" s="125"/>
       <c r="O3" s="125"/>
       <c r="P3" s="12"/>
     </row>
     <row r="4" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="198"/>
       <c r="M4" s="126"/>
       <c r="N4" s="126"/>
       <c r="O4" s="126"/>
       <c r="P4" s="12"/>
     </row>
     <row r="5" spans="2:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="226" t="s">
+      <c r="B5" s="235" t="s">
         <v>406</v>
       </c>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="227"/>
-      <c r="H5" s="227"/>
-      <c r="I5" s="227"/>
-      <c r="J5" s="227"/>
-      <c r="K5" s="227"/>
-      <c r="L5" s="228"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="236"/>
+      <c r="F5" s="236"/>
+      <c r="G5" s="236"/>
+      <c r="H5" s="236"/>
+      <c r="I5" s="236"/>
+      <c r="J5" s="236"/>
+      <c r="K5" s="236"/>
+      <c r="L5" s="237"/>
       <c r="M5" s="87"/>
       <c r="N5" s="87"/>
       <c r="O5" s="87"/>
       <c r="P5" s="12"/>
     </row>
     <row r="6" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="190"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="191"/>
-      <c r="E6" s="191"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="191"/>
-      <c r="H6" s="191"/>
-      <c r="I6" s="191"/>
-      <c r="J6" s="191"/>
-      <c r="K6" s="191"/>
-      <c r="L6" s="192"/>
+      <c r="B6" s="199"/>
+      <c r="C6" s="200"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="200"/>
+      <c r="K6" s="200"/>
+      <c r="L6" s="201"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
@@ -5869,12 +5891,12 @@
     <mergeCell ref="B5:L6"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:F15 E17 H9:O15">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>($C$21=2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>($C$21=2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5905,32 +5927,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="223" t="s">
+      <c r="B3" s="232" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="225"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
@@ -6008,11 +6030,144 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="161"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="162"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="164"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="162" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="163" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="163" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="162" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="163" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
+      <c r="K4" s="167">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="163" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="163" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="167">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="165" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="165" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="166">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:K6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>($C$15=1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -6026,84 +6181,84 @@
   <sheetData>
     <row r="1" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="191"/>
+      <c r="P2" s="191"/>
+      <c r="Q2" s="192"/>
     </row>
     <row r="3" spans="2:17" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>353</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="185"/>
-      <c r="P3" s="185"/>
-      <c r="Q3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="194"/>
+      <c r="O3" s="194"/>
+      <c r="P3" s="194"/>
+      <c r="Q3" s="195"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="188"/>
-      <c r="O4" s="188"/>
-      <c r="P4" s="188"/>
-      <c r="Q4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="197"/>
+      <c r="P4" s="197"/>
+      <c r="Q4" s="198"/>
     </row>
     <row r="5" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>352</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="191"/>
-      <c r="P5" s="191"/>
-      <c r="Q5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
+      <c r="O5" s="200"/>
+      <c r="P5" s="200"/>
+      <c r="Q5" s="201"/>
     </row>
     <row r="7" spans="2:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
@@ -6121,29 +6276,29 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="193" t="s">
+      <c r="E8" s="202" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="195" t="s">
+      <c r="F8" s="204" t="s">
         <v>162</v>
       </c>
-      <c r="G8" s="195" t="s">
+      <c r="G8" s="204" t="s">
         <v>163</v>
       </c>
-      <c r="H8" s="179" t="s">
+      <c r="H8" s="188" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="179" t="s">
+      <c r="I8" s="188" t="s">
         <v>274</v>
       </c>
-      <c r="J8" s="179"/>
-      <c r="K8" s="179"/>
-      <c r="L8" s="179"/>
-      <c r="M8" s="179"/>
-      <c r="N8" s="179"/>
-      <c r="O8" s="179"/>
-      <c r="P8" s="179"/>
-      <c r="Q8" s="180"/>
+      <c r="J8" s="188"/>
+      <c r="K8" s="188"/>
+      <c r="L8" s="188"/>
+      <c r="M8" s="188"/>
+      <c r="N8" s="188"/>
+      <c r="O8" s="188"/>
+      <c r="P8" s="188"/>
+      <c r="Q8" s="189"/>
     </row>
     <row r="9" spans="2:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
@@ -6152,10 +6307,10 @@
       <c r="C9" s="6">
         <v>100</v>
       </c>
-      <c r="E9" s="194"/>
-      <c r="F9" s="196"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="197"/>
+      <c r="E9" s="203"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="206"/>
       <c r="I9" s="103" t="s">
         <v>347</v>
       </c>
@@ -7611,60 +7766,60 @@
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
     </row>
     <row r="3" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>354</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="195"/>
     </row>
     <row r="4" spans="2:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="198"/>
     </row>
     <row r="5" spans="2:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="201"/>
     </row>
     <row r="7" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
@@ -7690,7 +7845,7 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="198" t="s">
+      <c r="E8" s="207" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -7708,7 +7863,7 @@
       <c r="J8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="201" t="s">
+      <c r="K8" s="210" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7719,7 +7874,7 @@
       <c r="C9" s="6">
         <v>120</v>
       </c>
-      <c r="E9" s="199"/>
+      <c r="E9" s="208"/>
       <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
@@ -7735,7 +7890,7 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="202"/>
+      <c r="K9" s="211"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
@@ -7744,7 +7899,7 @@
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="199"/>
+      <c r="E10" s="208"/>
       <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
@@ -7760,7 +7915,7 @@
       <c r="J10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="203"/>
+      <c r="K10" s="212"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -7770,7 +7925,7 @@
         <f>SUM(C8:C10)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="199"/>
+      <c r="E11" s="208"/>
       <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
@@ -7786,12 +7941,12 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="204" t="s">
+      <c r="K11" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="199"/>
+      <c r="E12" s="208"/>
       <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
@@ -7807,10 +7962,10 @@
       <c r="J12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="202"/>
+      <c r="K12" s="211"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="199"/>
+      <c r="E13" s="208"/>
       <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
@@ -7826,13 +7981,13 @@
       <c r="J13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K13" s="202"/>
+      <c r="K13" s="211"/>
     </row>
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="199"/>
+      <c r="E14" s="208"/>
       <c r="F14" s="2" t="s">
         <v>62</v>
       </c>
@@ -7848,7 +8003,7 @@
       <c r="J14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="202"/>
+      <c r="K14" s="211"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -7858,7 +8013,7 @@
         <f>'Principal - ABP'!F19</f>
         <v>0</v>
       </c>
-      <c r="E15" s="199"/>
+      <c r="E15" s="208"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -7874,7 +8029,7 @@
       <c r="J15" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="202"/>
+      <c r="K15" s="211"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -7884,7 +8039,7 @@
         <f>C9*C15</f>
         <v>0</v>
       </c>
-      <c r="E16" s="199"/>
+      <c r="E16" s="208"/>
       <c r="F16" s="2" t="s">
         <v>64</v>
       </c>
@@ -7900,7 +8055,7 @@
       <c r="J16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="203"/>
+      <c r="K16" s="212"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -7910,7 +8065,7 @@
         <f>(IF(C15=1,H21,IF(C15=2,H37,IF(C15=3,H55,IF(C15=4,H76,IF(C15=5,H97,H118))))))</f>
         <v>574</v>
       </c>
-      <c r="E17" s="199"/>
+      <c r="E17" s="208"/>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
@@ -7926,7 +8081,7 @@
       <c r="J17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="204" t="s">
+      <c r="K17" s="213" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7938,7 +8093,7 @@
         <f>C17/C16-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E18" s="199"/>
+      <c r="E18" s="208"/>
       <c r="F18" s="2" t="s">
         <v>66</v>
       </c>
@@ -7954,7 +8109,7 @@
       <c r="J18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K18" s="202"/>
+      <c r="K18" s="211"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -7964,7 +8119,7 @@
         <f>C15*10</f>
         <v>0</v>
       </c>
-      <c r="E19" s="199"/>
+      <c r="E19" s="208"/>
       <c r="F19" s="2" t="s">
         <v>67</v>
       </c>
@@ -7980,7 +8135,7 @@
       <c r="J19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="202"/>
+      <c r="K19" s="211"/>
     </row>
     <row r="20" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
@@ -7990,7 +8145,7 @@
         <f>IF(C15=1,I21,IF(C15=2,I37,IF(C15=3,I55,IF(C15=4,I76,IF(C15=5,I97,I118)))))</f>
         <v>60.000000000000007</v>
       </c>
-      <c r="E20" s="200"/>
+      <c r="E20" s="209"/>
       <c r="F20" s="4" t="s">
         <v>68</v>
       </c>
@@ -8006,7 +8161,7 @@
       <c r="J20" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="205"/>
+      <c r="K20" s="214"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
@@ -8033,7 +8188,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="198" t="s">
+      <c r="E23" s="207" t="s">
         <v>141</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -8051,12 +8206,12 @@
       <c r="J23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="201" t="s">
+      <c r="K23" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="199"/>
+      <c r="E24" s="208"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
@@ -8072,10 +8227,10 @@
       <c r="J24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="202"/>
+      <c r="K24" s="211"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="199"/>
+      <c r="E25" s="208"/>
       <c r="F25" s="2" t="s">
         <v>58</v>
       </c>
@@ -8091,10 +8246,10 @@
       <c r="J25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K25" s="203"/>
+      <c r="K25" s="212"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="199"/>
+      <c r="E26" s="208"/>
       <c r="F26" s="2" t="s">
         <v>59</v>
       </c>
@@ -8110,12 +8265,12 @@
       <c r="J26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="204" t="s">
+      <c r="K26" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="199"/>
+      <c r="E27" s="208"/>
       <c r="F27" s="2" t="s">
         <v>60</v>
       </c>
@@ -8131,10 +8286,10 @@
       <c r="J27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="202"/>
+      <c r="K27" s="211"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="199"/>
+      <c r="E28" s="208"/>
       <c r="F28" s="2" t="s">
         <v>61</v>
       </c>
@@ -8150,10 +8305,10 @@
       <c r="J28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="202"/>
+      <c r="K28" s="211"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="199"/>
+      <c r="E29" s="208"/>
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
@@ -8169,10 +8324,10 @@
       <c r="J29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="202"/>
+      <c r="K29" s="211"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="199"/>
+      <c r="E30" s="208"/>
       <c r="F30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8188,10 +8343,10 @@
       <c r="J30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="202"/>
+      <c r="K30" s="211"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="199"/>
+      <c r="E31" s="208"/>
       <c r="F31" s="2" t="s">
         <v>64</v>
       </c>
@@ -8207,10 +8362,10 @@
       <c r="J31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K31" s="202"/>
+      <c r="K31" s="211"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="199"/>
+      <c r="E32" s="208"/>
       <c r="F32" s="2" t="s">
         <v>65</v>
       </c>
@@ -8226,10 +8381,10 @@
       <c r="J32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="203"/>
+      <c r="K32" s="212"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E33" s="199"/>
+      <c r="E33" s="208"/>
       <c r="F33" s="2" t="s">
         <v>66</v>
       </c>
@@ -8245,12 +8400,12 @@
       <c r="J33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K33" s="204" t="s">
+      <c r="K33" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" s="199"/>
+      <c r="E34" s="208"/>
       <c r="F34" s="2" t="s">
         <v>67</v>
       </c>
@@ -8266,10 +8421,10 @@
       <c r="J34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K34" s="202"/>
+      <c r="K34" s="211"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E35" s="199"/>
+      <c r="E35" s="208"/>
       <c r="F35" s="2" t="s">
         <v>68</v>
       </c>
@@ -8285,10 +8440,10 @@
       <c r="J35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K35" s="202"/>
+      <c r="K35" s="211"/>
     </row>
     <row r="36" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="200"/>
+      <c r="E36" s="209"/>
       <c r="F36" s="4" t="s">
         <v>69</v>
       </c>
@@ -8304,7 +8459,7 @@
       <c r="J36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K36" s="205"/>
+      <c r="K36" s="214"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
@@ -8331,7 +8486,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E39" s="198" t="s">
+      <c r="E39" s="207" t="s">
         <v>142</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -8349,12 +8504,12 @@
       <c r="J39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K39" s="201" t="s">
+      <c r="K39" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E40" s="199"/>
+      <c r="E40" s="208"/>
       <c r="F40" s="2" t="s">
         <v>57</v>
       </c>
@@ -8370,10 +8525,10 @@
       <c r="J40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K40" s="202"/>
+      <c r="K40" s="211"/>
     </row>
     <row r="41" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E41" s="199"/>
+      <c r="E41" s="208"/>
       <c r="F41" s="2" t="s">
         <v>58</v>
       </c>
@@ -8389,10 +8544,10 @@
       <c r="J41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K41" s="203"/>
+      <c r="K41" s="212"/>
     </row>
     <row r="42" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E42" s="199"/>
+      <c r="E42" s="208"/>
       <c r="F42" s="2" t="s">
         <v>59</v>
       </c>
@@ -8408,12 +8563,12 @@
       <c r="J42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K42" s="204" t="s">
+      <c r="K42" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E43" s="199"/>
+      <c r="E43" s="208"/>
       <c r="F43" s="2" t="s">
         <v>60</v>
       </c>
@@ -8429,10 +8584,10 @@
       <c r="J43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K43" s="202"/>
+      <c r="K43" s="211"/>
     </row>
     <row r="44" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E44" s="199"/>
+      <c r="E44" s="208"/>
       <c r="F44" s="2" t="s">
         <v>61</v>
       </c>
@@ -8448,10 +8603,10 @@
       <c r="J44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K44" s="202"/>
+      <c r="K44" s="211"/>
     </row>
     <row r="45" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E45" s="199"/>
+      <c r="E45" s="208"/>
       <c r="F45" s="2" t="s">
         <v>62</v>
       </c>
@@ -8467,10 +8622,10 @@
       <c r="J45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K45" s="202"/>
+      <c r="K45" s="211"/>
     </row>
     <row r="46" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E46" s="199"/>
+      <c r="E46" s="208"/>
       <c r="F46" s="2" t="s">
         <v>63</v>
       </c>
@@ -8486,10 +8641,10 @@
       <c r="J46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K46" s="202"/>
+      <c r="K46" s="211"/>
     </row>
     <row r="47" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E47" s="199"/>
+      <c r="E47" s="208"/>
       <c r="F47" s="2" t="s">
         <v>64</v>
       </c>
@@ -8505,10 +8660,10 @@
       <c r="J47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K47" s="202"/>
+      <c r="K47" s="211"/>
     </row>
     <row r="48" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E48" s="199"/>
+      <c r="E48" s="208"/>
       <c r="F48" s="2" t="s">
         <v>65</v>
       </c>
@@ -8524,10 +8679,10 @@
       <c r="J48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K48" s="202"/>
+      <c r="K48" s="211"/>
     </row>
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E49" s="199"/>
+      <c r="E49" s="208"/>
       <c r="F49" s="2" t="s">
         <v>66</v>
       </c>
@@ -8543,10 +8698,10 @@
       <c r="J49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K49" s="202"/>
+      <c r="K49" s="211"/>
     </row>
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E50" s="199"/>
+      <c r="E50" s="208"/>
       <c r="F50" s="2" t="s">
         <v>67</v>
       </c>
@@ -8562,10 +8717,10 @@
       <c r="J50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K50" s="203"/>
+      <c r="K50" s="212"/>
     </row>
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E51" s="199"/>
+      <c r="E51" s="208"/>
       <c r="F51" s="2" t="s">
         <v>68</v>
       </c>
@@ -8581,12 +8736,12 @@
       <c r="J51" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K51" s="204" t="s">
+      <c r="K51" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E52" s="199"/>
+      <c r="E52" s="208"/>
       <c r="F52" s="2" t="s">
         <v>69</v>
       </c>
@@ -8602,10 +8757,10 @@
       <c r="J52" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K52" s="202"/>
+      <c r="K52" s="211"/>
     </row>
     <row r="53" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E53" s="199"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="2" t="s">
         <v>70</v>
       </c>
@@ -8621,10 +8776,10 @@
       <c r="J53" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K53" s="202"/>
+      <c r="K53" s="211"/>
     </row>
     <row r="54" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="200"/>
+      <c r="E54" s="209"/>
       <c r="F54" s="4" t="s">
         <v>71</v>
       </c>
@@ -8640,7 +8795,7 @@
       <c r="J54" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K54" s="205"/>
+      <c r="K54" s="214"/>
     </row>
     <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
@@ -8667,7 +8822,7 @@
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E57" s="198" t="s">
+      <c r="E57" s="207" t="s">
         <v>143</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -8685,12 +8840,12 @@
       <c r="J57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K57" s="201" t="s">
+      <c r="K57" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E58" s="199"/>
+      <c r="E58" s="208"/>
       <c r="F58" s="2" t="s">
         <v>57</v>
       </c>
@@ -8706,10 +8861,10 @@
       <c r="J58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K58" s="202"/>
+      <c r="K58" s="211"/>
     </row>
     <row r="59" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E59" s="199"/>
+      <c r="E59" s="208"/>
       <c r="F59" s="2" t="s">
         <v>58</v>
       </c>
@@ -8725,10 +8880,10 @@
       <c r="J59" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K59" s="203"/>
+      <c r="K59" s="212"/>
     </row>
     <row r="60" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E60" s="199"/>
+      <c r="E60" s="208"/>
       <c r="F60" s="2" t="s">
         <v>59</v>
       </c>
@@ -8744,12 +8899,12 @@
       <c r="J60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K60" s="204" t="s">
+      <c r="K60" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E61" s="199"/>
+      <c r="E61" s="208"/>
       <c r="F61" s="2" t="s">
         <v>60</v>
       </c>
@@ -8765,10 +8920,10 @@
       <c r="J61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K61" s="202"/>
+      <c r="K61" s="211"/>
     </row>
     <row r="62" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E62" s="199"/>
+      <c r="E62" s="208"/>
       <c r="F62" s="2" t="s">
         <v>61</v>
       </c>
@@ -8784,10 +8939,10 @@
       <c r="J62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K62" s="202"/>
+      <c r="K62" s="211"/>
     </row>
     <row r="63" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E63" s="199"/>
+      <c r="E63" s="208"/>
       <c r="F63" s="2" t="s">
         <v>62</v>
       </c>
@@ -8803,10 +8958,10 @@
       <c r="J63" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K63" s="202"/>
+      <c r="K63" s="211"/>
     </row>
     <row r="64" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="199"/>
+      <c r="E64" s="208"/>
       <c r="F64" s="2" t="s">
         <v>63</v>
       </c>
@@ -8822,10 +8977,10 @@
       <c r="J64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K64" s="202"/>
+      <c r="K64" s="211"/>
     </row>
     <row r="65" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E65" s="199"/>
+      <c r="E65" s="208"/>
       <c r="F65" s="2" t="s">
         <v>64</v>
       </c>
@@ -8841,10 +8996,10 @@
       <c r="J65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K65" s="202"/>
+      <c r="K65" s="211"/>
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E66" s="199"/>
+      <c r="E66" s="208"/>
       <c r="F66" s="2" t="s">
         <v>65</v>
       </c>
@@ -8860,10 +9015,10 @@
       <c r="J66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K66" s="202"/>
+      <c r="K66" s="211"/>
     </row>
     <row r="67" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E67" s="199"/>
+      <c r="E67" s="208"/>
       <c r="F67" s="2" t="s">
         <v>66</v>
       </c>
@@ -8879,10 +9034,10 @@
       <c r="J67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K67" s="202"/>
+      <c r="K67" s="211"/>
     </row>
     <row r="68" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E68" s="199"/>
+      <c r="E68" s="208"/>
       <c r="F68" s="2" t="s">
         <v>67</v>
       </c>
@@ -8898,10 +9053,10 @@
       <c r="J68" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K68" s="202"/>
+      <c r="K68" s="211"/>
     </row>
     <row r="69" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E69" s="199"/>
+      <c r="E69" s="208"/>
       <c r="F69" s="2" t="s">
         <v>68</v>
       </c>
@@ -8917,10 +9072,10 @@
       <c r="J69" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K69" s="202"/>
+      <c r="K69" s="211"/>
     </row>
     <row r="70" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E70" s="199"/>
+      <c r="E70" s="208"/>
       <c r="F70" s="2" t="s">
         <v>69</v>
       </c>
@@ -8936,10 +9091,10 @@
       <c r="J70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K70" s="202"/>
+      <c r="K70" s="211"/>
     </row>
     <row r="71" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E71" s="199"/>
+      <c r="E71" s="208"/>
       <c r="F71" s="2" t="s">
         <v>70</v>
       </c>
@@ -8955,10 +9110,10 @@
       <c r="J71" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K71" s="203"/>
+      <c r="K71" s="212"/>
     </row>
     <row r="72" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E72" s="199"/>
+      <c r="E72" s="208"/>
       <c r="F72" s="2" t="s">
         <v>71</v>
       </c>
@@ -8974,12 +9129,12 @@
       <c r="J72" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K72" s="204" t="s">
+      <c r="K72" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E73" s="199"/>
+      <c r="E73" s="208"/>
       <c r="F73" s="2" t="s">
         <v>72</v>
       </c>
@@ -8995,10 +9150,10 @@
       <c r="J73" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K73" s="202"/>
+      <c r="K73" s="211"/>
     </row>
     <row r="74" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E74" s="199"/>
+      <c r="E74" s="208"/>
       <c r="F74" s="2" t="s">
         <v>73</v>
       </c>
@@ -9014,10 +9169,10 @@
       <c r="J74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K74" s="202"/>
+      <c r="K74" s="211"/>
     </row>
     <row r="75" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E75" s="200"/>
+      <c r="E75" s="209"/>
       <c r="F75" s="4" t="s">
         <v>74</v>
       </c>
@@ -9033,7 +9188,7 @@
       <c r="J75" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K75" s="205"/>
+      <c r="K75" s="214"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
@@ -9053,7 +9208,7 @@
     </row>
     <row r="77" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E78" s="198" t="s">
+      <c r="E78" s="207" t="s">
         <v>144</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -9071,12 +9226,12 @@
       <c r="J78" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K78" s="206" t="s">
+      <c r="K78" s="215" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E79" s="199"/>
+      <c r="E79" s="208"/>
       <c r="F79" s="2" t="s">
         <v>57</v>
       </c>
@@ -9092,10 +9247,10 @@
       <c r="J79" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K79" s="207"/>
+      <c r="K79" s="216"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E80" s="199"/>
+      <c r="E80" s="208"/>
       <c r="F80" s="2" t="s">
         <v>58</v>
       </c>
@@ -9111,10 +9266,10 @@
       <c r="J80" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K80" s="208"/>
+      <c r="K80" s="217"/>
     </row>
     <row r="81" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E81" s="199"/>
+      <c r="E81" s="208"/>
       <c r="F81" s="2" t="s">
         <v>59</v>
       </c>
@@ -9130,12 +9285,12 @@
       <c r="J81" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K81" s="204" t="s">
+      <c r="K81" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E82" s="199"/>
+      <c r="E82" s="208"/>
       <c r="F82" s="2" t="s">
         <v>60</v>
       </c>
@@ -9151,10 +9306,10 @@
       <c r="J82" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K82" s="202"/>
+      <c r="K82" s="211"/>
     </row>
     <row r="83" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E83" s="199"/>
+      <c r="E83" s="208"/>
       <c r="F83" s="2" t="s">
         <v>61</v>
       </c>
@@ -9170,10 +9325,10 @@
       <c r="J83" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K83" s="202"/>
+      <c r="K83" s="211"/>
     </row>
     <row r="84" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E84" s="199"/>
+      <c r="E84" s="208"/>
       <c r="F84" s="2" t="s">
         <v>62</v>
       </c>
@@ -9189,10 +9344,10 @@
       <c r="J84" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K84" s="202"/>
+      <c r="K84" s="211"/>
     </row>
     <row r="85" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E85" s="199"/>
+      <c r="E85" s="208"/>
       <c r="F85" s="2" t="s">
         <v>63</v>
       </c>
@@ -9208,10 +9363,10 @@
       <c r="J85" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K85" s="202"/>
+      <c r="K85" s="211"/>
     </row>
     <row r="86" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E86" s="199"/>
+      <c r="E86" s="208"/>
       <c r="F86" s="2" t="s">
         <v>64</v>
       </c>
@@ -9227,10 +9382,10 @@
       <c r="J86" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K86" s="202"/>
+      <c r="K86" s="211"/>
     </row>
     <row r="87" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E87" s="199"/>
+      <c r="E87" s="208"/>
       <c r="F87" s="2" t="s">
         <v>65</v>
       </c>
@@ -9246,10 +9401,10 @@
       <c r="J87" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K87" s="202"/>
+      <c r="K87" s="211"/>
     </row>
     <row r="88" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E88" s="199"/>
+      <c r="E88" s="208"/>
       <c r="F88" s="2" t="s">
         <v>66</v>
       </c>
@@ -9265,10 +9420,10 @@
       <c r="J88" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K88" s="202"/>
+      <c r="K88" s="211"/>
     </row>
     <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="199"/>
+      <c r="E89" s="208"/>
       <c r="F89" s="2" t="s">
         <v>67</v>
       </c>
@@ -9284,10 +9439,10 @@
       <c r="J89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K89" s="202"/>
+      <c r="K89" s="211"/>
     </row>
     <row r="90" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E90" s="199"/>
+      <c r="E90" s="208"/>
       <c r="F90" s="2" t="s">
         <v>68</v>
       </c>
@@ -9303,10 +9458,10 @@
       <c r="J90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K90" s="202"/>
+      <c r="K90" s="211"/>
     </row>
     <row r="91" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E91" s="199"/>
+      <c r="E91" s="208"/>
       <c r="F91" s="2" t="s">
         <v>69</v>
       </c>
@@ -9322,10 +9477,10 @@
       <c r="J91" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K91" s="202"/>
+      <c r="K91" s="211"/>
     </row>
     <row r="92" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E92" s="199"/>
+      <c r="E92" s="208"/>
       <c r="F92" s="2" t="s">
         <v>70</v>
       </c>
@@ -9341,10 +9496,10 @@
       <c r="J92" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K92" s="202"/>
+      <c r="K92" s="211"/>
     </row>
     <row r="93" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E93" s="199"/>
+      <c r="E93" s="208"/>
       <c r="F93" s="2" t="s">
         <v>71</v>
       </c>
@@ -9360,10 +9515,10 @@
       <c r="J93" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K93" s="203"/>
+      <c r="K93" s="212"/>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E94" s="199"/>
+      <c r="E94" s="208"/>
       <c r="F94" s="2" t="s">
         <v>72</v>
       </c>
@@ -9379,12 +9534,12 @@
       <c r="J94" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K94" s="204" t="s">
+      <c r="K94" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E95" s="199"/>
+      <c r="E95" s="208"/>
       <c r="F95" s="2" t="s">
         <v>73</v>
       </c>
@@ -9400,10 +9555,10 @@
       <c r="J95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K95" s="202"/>
+      <c r="K95" s="211"/>
     </row>
     <row r="96" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E96" s="200"/>
+      <c r="E96" s="209"/>
       <c r="F96" s="4" t="s">
         <v>74</v>
       </c>
@@ -9419,7 +9574,7 @@
       <c r="J96" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K96" s="205"/>
+      <c r="K96" s="214"/>
     </row>
     <row r="97" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
@@ -9439,7 +9594,7 @@
     </row>
     <row r="98" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E99" s="198" t="s">
+      <c r="E99" s="207" t="s">
         <v>145</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -9457,12 +9612,12 @@
       <c r="J99" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K99" s="201" t="s">
+      <c r="K99" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="100" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E100" s="199"/>
+      <c r="E100" s="208"/>
       <c r="F100" s="2" t="s">
         <v>57</v>
       </c>
@@ -9478,10 +9633,10 @@
       <c r="J100" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K100" s="202"/>
+      <c r="K100" s="211"/>
     </row>
     <row r="101" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E101" s="199"/>
+      <c r="E101" s="208"/>
       <c r="F101" s="2" t="s">
         <v>58</v>
       </c>
@@ -9497,10 +9652,10 @@
       <c r="J101" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K101" s="203"/>
+      <c r="K101" s="212"/>
     </row>
     <row r="102" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E102" s="199"/>
+      <c r="E102" s="208"/>
       <c r="F102" s="2" t="s">
         <v>59</v>
       </c>
@@ -9516,12 +9671,12 @@
       <c r="J102" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K102" s="204" t="s">
+      <c r="K102" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="103" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E103" s="199"/>
+      <c r="E103" s="208"/>
       <c r="F103" s="2" t="s">
         <v>60</v>
       </c>
@@ -9537,10 +9692,10 @@
       <c r="J103" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K103" s="202"/>
+      <c r="K103" s="211"/>
     </row>
     <row r="104" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E104" s="199"/>
+      <c r="E104" s="208"/>
       <c r="F104" s="2" t="s">
         <v>61</v>
       </c>
@@ -9556,10 +9711,10 @@
       <c r="J104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K104" s="202"/>
+      <c r="K104" s="211"/>
     </row>
     <row r="105" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E105" s="199"/>
+      <c r="E105" s="208"/>
       <c r="F105" s="2" t="s">
         <v>62</v>
       </c>
@@ -9575,10 +9730,10 @@
       <c r="J105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K105" s="202"/>
+      <c r="K105" s="211"/>
     </row>
     <row r="106" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E106" s="199"/>
+      <c r="E106" s="208"/>
       <c r="F106" s="2" t="s">
         <v>63</v>
       </c>
@@ -9594,10 +9749,10 @@
       <c r="J106" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K106" s="202"/>
+      <c r="K106" s="211"/>
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E107" s="199"/>
+      <c r="E107" s="208"/>
       <c r="F107" s="2" t="s">
         <v>64</v>
       </c>
@@ -9613,10 +9768,10 @@
       <c r="J107" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K107" s="202"/>
+      <c r="K107" s="211"/>
     </row>
     <row r="108" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E108" s="199"/>
+      <c r="E108" s="208"/>
       <c r="F108" s="2" t="s">
         <v>65</v>
       </c>
@@ -9632,10 +9787,10 @@
       <c r="J108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K108" s="202"/>
+      <c r="K108" s="211"/>
     </row>
     <row r="109" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E109" s="199"/>
+      <c r="E109" s="208"/>
       <c r="F109" s="2" t="s">
         <v>66</v>
       </c>
@@ -9651,10 +9806,10 @@
       <c r="J109" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K109" s="202"/>
+      <c r="K109" s="211"/>
     </row>
     <row r="110" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E110" s="199"/>
+      <c r="E110" s="208"/>
       <c r="F110" s="2" t="s">
         <v>67</v>
       </c>
@@ -9670,10 +9825,10 @@
       <c r="J110" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K110" s="202"/>
+      <c r="K110" s="211"/>
     </row>
     <row r="111" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E111" s="199"/>
+      <c r="E111" s="208"/>
       <c r="F111" s="2" t="s">
         <v>68</v>
       </c>
@@ -9689,10 +9844,10 @@
       <c r="J111" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K111" s="202"/>
+      <c r="K111" s="211"/>
     </row>
     <row r="112" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E112" s="199"/>
+      <c r="E112" s="208"/>
       <c r="F112" s="2" t="s">
         <v>69</v>
       </c>
@@ -9708,10 +9863,10 @@
       <c r="J112" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K112" s="202"/>
+      <c r="K112" s="211"/>
     </row>
     <row r="113" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E113" s="199"/>
+      <c r="E113" s="208"/>
       <c r="F113" s="2" t="s">
         <v>70</v>
       </c>
@@ -9727,10 +9882,10 @@
       <c r="J113" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K113" s="202"/>
+      <c r="K113" s="211"/>
     </row>
     <row r="114" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E114" s="199"/>
+      <c r="E114" s="208"/>
       <c r="F114" s="2" t="s">
         <v>71</v>
       </c>
@@ -9746,10 +9901,10 @@
       <c r="J114" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K114" s="202"/>
+      <c r="K114" s="211"/>
     </row>
     <row r="115" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E115" s="199"/>
+      <c r="E115" s="208"/>
       <c r="F115" s="2" t="s">
         <v>72</v>
       </c>
@@ -9765,10 +9920,10 @@
       <c r="J115" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K115" s="203"/>
+      <c r="K115" s="212"/>
     </row>
     <row r="116" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E116" s="199"/>
+      <c r="E116" s="208"/>
       <c r="F116" s="2" t="s">
         <v>73</v>
       </c>
@@ -9784,12 +9939,12 @@
       <c r="J116" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K116" s="204" t="s">
+      <c r="K116" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="200"/>
+      <c r="E117" s="209"/>
       <c r="F117" s="4" t="s">
         <v>74</v>
       </c>
@@ -9805,7 +9960,7 @@
       <c r="J117" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K117" s="205"/>
+      <c r="K117" s="214"/>
     </row>
     <row r="118" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F118" s="1"/>
@@ -9856,32 +10011,32 @@
     <mergeCell ref="E78:E96"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:K21">
-    <cfRule type="expression" dxfId="62" priority="7">
+    <cfRule type="expression" dxfId="63" priority="7">
       <formula>($C$15=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:K37">
-    <cfRule type="expression" dxfId="61" priority="6">
+    <cfRule type="expression" dxfId="62" priority="6">
       <formula>($C$15=2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:K55">
-    <cfRule type="expression" dxfId="60" priority="5">
+    <cfRule type="expression" dxfId="61" priority="5">
       <formula>($C$15=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57:K76">
-    <cfRule type="expression" dxfId="59" priority="4">
+    <cfRule type="expression" dxfId="60" priority="4">
       <formula>($C$15=4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E78:K97">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="59" priority="2">
       <formula>($C$15=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99:K118">
-    <cfRule type="expression" dxfId="57" priority="1">
+    <cfRule type="expression" dxfId="58" priority="1">
       <formula>($C$15=6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9918,105 +10073,105 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="192"/>
     </row>
     <row r="3" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="210" t="s">
+      <c r="B3" s="219" t="s">
         <v>356</v>
       </c>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="211"/>
-      <c r="F3" s="211"/>
-      <c r="G3" s="211"/>
-      <c r="H3" s="211"/>
-      <c r="I3" s="211"/>
-      <c r="J3" s="211"/>
-      <c r="K3" s="211"/>
-      <c r="L3" s="211"/>
-      <c r="M3" s="211"/>
-      <c r="N3" s="212"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="220"/>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
+      <c r="K3" s="220"/>
+      <c r="L3" s="220"/>
+      <c r="M3" s="220"/>
+      <c r="N3" s="221"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="198"/>
     </row>
     <row r="5" spans="2:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>408</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="201"/>
     </row>
     <row r="7" spans="2:15" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="213" t="s">
+      <c r="E7" s="222" t="s">
         <v>205</v>
       </c>
-      <c r="F7" s="213" t="s">
+      <c r="F7" s="222" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="213" t="s">
+      <c r="G7" s="222" t="s">
         <v>162</v>
       </c>
-      <c r="H7" s="213" t="s">
+      <c r="H7" s="222" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="209" t="s">
+      <c r="I7" s="218" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="209" t="s">
+      <c r="J7" s="218" t="s">
         <v>206</v>
       </c>
-      <c r="K7" s="209" t="s">
+      <c r="K7" s="218" t="s">
         <v>207</v>
       </c>
-      <c r="L7" s="209" t="s">
+      <c r="L7" s="218" t="s">
         <v>208</v>
       </c>
-      <c r="M7" s="209" t="s">
+      <c r="M7" s="218" t="s">
         <v>209</v>
       </c>
-      <c r="N7" s="209" t="s">
+      <c r="N7" s="218" t="s">
         <v>210</v>
       </c>
     </row>
@@ -10027,16 +10182,16 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="213"/>
-      <c r="F8" s="213"/>
-      <c r="G8" s="213"/>
-      <c r="H8" s="213"/>
-      <c r="I8" s="209"/>
-      <c r="J8" s="209"/>
-      <c r="K8" s="209"/>
-      <c r="L8" s="209"/>
-      <c r="M8" s="209"/>
-      <c r="N8" s="209"/>
+      <c r="E8" s="222"/>
+      <c r="F8" s="222"/>
+      <c r="G8" s="222"/>
+      <c r="H8" s="222"/>
+      <c r="I8" s="218"/>
+      <c r="J8" s="218"/>
+      <c r="K8" s="218"/>
+      <c r="L8" s="218"/>
+      <c r="M8" s="218"/>
+      <c r="N8" s="218"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
@@ -11084,178 +11239,178 @@
     <mergeCell ref="H7:H8"/>
   </mergeCells>
   <conditionalFormatting sqref="E9 G9:N9">
-    <cfRule type="expression" dxfId="56" priority="41">
+    <cfRule type="expression" dxfId="57" priority="41">
       <formula>NOT(ISBLANK($E$9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:N10 F9">
-    <cfRule type="expression" dxfId="55" priority="39">
+    <cfRule type="expression" dxfId="56" priority="39">
       <formula>NOT(ISBLANK($E$10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:N11">
-    <cfRule type="expression" dxfId="54" priority="37">
+    <cfRule type="expression" dxfId="55" priority="37">
       <formula>NOT(ISBLANK($E$11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:N12">
-    <cfRule type="expression" dxfId="53" priority="36">
+    <cfRule type="expression" dxfId="54" priority="36">
       <formula>NOT(ISBLANK($E$12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13:N13">
-    <cfRule type="expression" dxfId="52" priority="34">
+    <cfRule type="expression" dxfId="53" priority="34">
       <formula>NOT(ISBLANK($E$13))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:N14">
-    <cfRule type="expression" dxfId="51" priority="33">
+    <cfRule type="expression" dxfId="52" priority="33">
       <formula>NOT(ISBLANK($E$14))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:N15">
-    <cfRule type="expression" dxfId="50" priority="32">
+    <cfRule type="expression" dxfId="51" priority="32">
       <formula>NOT(ISBLANK($E$15))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:N16">
-    <cfRule type="expression" dxfId="49" priority="31">
+    <cfRule type="expression" dxfId="50" priority="31">
       <formula>NOT(ISBLANK($E$16))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:N17">
-    <cfRule type="expression" dxfId="48" priority="30">
+    <cfRule type="expression" dxfId="49" priority="30">
       <formula>NOT(ISBLANK($E$17))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:N18">
-    <cfRule type="expression" dxfId="47" priority="29">
+    <cfRule type="expression" dxfId="48" priority="29">
       <formula>NOT(ISBLANK($E$18))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:N19">
-    <cfRule type="expression" dxfId="46" priority="28">
+    <cfRule type="expression" dxfId="47" priority="28">
       <formula>NOT(ISBLANK($E$19))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:N20">
-    <cfRule type="expression" dxfId="45" priority="27">
+    <cfRule type="expression" dxfId="46" priority="27">
       <formula>NOT(ISBLANK($E$20))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:N21">
-    <cfRule type="expression" dxfId="44" priority="26">
+    <cfRule type="expression" dxfId="45" priority="26">
       <formula>NOT(ISBLANK($E$21))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:N22">
-    <cfRule type="expression" dxfId="43" priority="25">
+    <cfRule type="expression" dxfId="44" priority="25">
       <formula>NOT(ISBLANK($E$22))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:N23">
-    <cfRule type="expression" dxfId="42" priority="24">
+    <cfRule type="expression" dxfId="43" priority="24">
       <formula>NOT(ISBLANK($E$23))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:N24">
-    <cfRule type="expression" dxfId="41" priority="23">
+    <cfRule type="expression" dxfId="42" priority="23">
       <formula>NOT(ISBLANK($E$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25:N25">
-    <cfRule type="expression" dxfId="40" priority="22">
+    <cfRule type="expression" dxfId="41" priority="22">
       <formula>NOT(ISBLANK($E$25))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:N26">
-    <cfRule type="expression" dxfId="39" priority="21">
+    <cfRule type="expression" dxfId="40" priority="21">
       <formula>NOT(ISBLANK($E$26))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27:N27">
-    <cfRule type="expression" dxfId="38" priority="19">
+    <cfRule type="expression" dxfId="39" priority="19">
       <formula>NOT(ISBLANK($E$27))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:N28">
-    <cfRule type="expression" dxfId="37" priority="18">
+    <cfRule type="expression" dxfId="38" priority="18">
       <formula>NOT(ISBLANK($E$28))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:N29">
-    <cfRule type="expression" dxfId="36" priority="17">
+    <cfRule type="expression" dxfId="37" priority="17">
       <formula>NOT(ISBLANK($E$29))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:N30">
-    <cfRule type="expression" dxfId="35" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>NOT(ISBLANK($E$30))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:N31">
-    <cfRule type="expression" dxfId="34" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>NOT(ISBLANK($E$31))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E32:N32">
-    <cfRule type="expression" dxfId="33" priority="14">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>NOT(ISBLANK($E$32))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:N33">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>NOT(ISBLANK($E$33))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:N34">
-    <cfRule type="expression" dxfId="31" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>NOT(ISBLANK($E$34))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:N35">
-    <cfRule type="expression" dxfId="30" priority="11">
+    <cfRule type="expression" dxfId="31" priority="11">
       <formula>NOT(ISBLANK($E$35))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36:N36">
-    <cfRule type="expression" dxfId="29" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>NOT(ISBLANK($E$36))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:N37">
-    <cfRule type="expression" dxfId="28" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>NOT(ISBLANK($E$37))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:N38">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>NOT(ISBLANK($E$38))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39:N39">
-    <cfRule type="expression" dxfId="26" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>NOT(ISBLANK($E$39))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:N40">
-    <cfRule type="expression" dxfId="25" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>NOT(ISBLANK($E$40))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>NOT(OR($C$17&lt;0.75*$C$16,$C$17&gt;1.25*$C$16))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>OR($C$17&lt;0.75*$C$16,$C$17&gt;1.25*$C$16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>($C$20=$C$19)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$C$20&lt;&gt;$C$19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11290,76 +11445,76 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="192"/>
     </row>
     <row r="3" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="194"/>
+      <c r="O3" s="195"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="188"/>
-      <c r="O4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="198"/>
     </row>
     <row r="5" spans="2:15" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
+      <c r="O5" s="201"/>
     </row>
     <row r="6" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -12165,27 +12320,27 @@
     <mergeCell ref="B5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:O7">
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>($C$15=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:O16">
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>($C$15=2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:O28">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>($C$15=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:O43">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>OR($C$15=4,$C$15=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:O45">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>($C$15=6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12203,8 +12358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12215,76 +12370,76 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="192"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="194"/>
+      <c r="O3" s="195"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="188"/>
-      <c r="O4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="198"/>
     </row>
     <row r="5" spans="2:15" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
+      <c r="O5" s="201"/>
     </row>
     <row r="6" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:15" ht="21" x14ac:dyDescent="0.25">
@@ -13380,32 +13535,32 @@
     <mergeCell ref="B5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:O12">
-    <cfRule type="expression" dxfId="15" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>($C$15=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:O20">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>($C$15=2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:O29">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="14" priority="4">
       <formula>($C$15=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:O39">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>($C$15=4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:O50">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>($C$15=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:O62">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>($C$15=6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13440,72 +13595,72 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
       <c r="L2" s="86"/>
       <c r="M2" s="86"/>
       <c r="N2" s="86"/>
       <c r="O2" s="86"/>
     </row>
     <row r="3" spans="2:15" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="184" t="s">
+      <c r="B3" s="193" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="186"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="195"/>
       <c r="L3" s="87"/>
       <c r="M3" s="87"/>
       <c r="N3" s="87"/>
       <c r="O3" s="87"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="198"/>
       <c r="L4" s="87"/>
       <c r="M4" s="87"/>
       <c r="N4" s="87"/>
       <c r="O4" s="87"/>
     </row>
     <row r="5" spans="2:15" ht="33.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="201"/>
       <c r="L5" s="87"/>
       <c r="M5" s="87"/>
       <c r="N5" s="87"/>
@@ -13557,10 +13712,10 @@
       <c r="C10" s="6">
         <v>20</v>
       </c>
-      <c r="E10" s="214" t="s">
+      <c r="E10" s="223" t="s">
         <v>247</v>
       </c>
-      <c r="F10" s="218" t="s">
+      <c r="F10" s="227" t="s">
         <v>409</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -13589,8 +13744,8 @@
         <f>SUM(C8:C10)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="215"/>
-      <c r="F11" s="219"/>
+      <c r="E11" s="224"/>
+      <c r="F11" s="228"/>
       <c r="G11" s="6" t="s">
         <v>249</v>
       </c>
@@ -13610,8 +13765,8 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E12" s="215"/>
-      <c r="F12" s="219"/>
+      <c r="E12" s="224"/>
+      <c r="F12" s="228"/>
       <c r="G12" s="6" t="s">
         <v>250</v>
       </c>
@@ -13637,8 +13792,8 @@
       <c r="C13" s="154">
         <v>10</v>
       </c>
-      <c r="E13" s="215"/>
-      <c r="F13" s="220"/>
+      <c r="E13" s="224"/>
+      <c r="F13" s="229"/>
       <c r="G13" s="6" t="s">
         <v>251</v>
       </c>
@@ -13664,8 +13819,8 @@
       <c r="C14" s="154">
         <v>1</v>
       </c>
-      <c r="E14" s="215"/>
-      <c r="F14" s="221" t="s">
+      <c r="E14" s="224"/>
+      <c r="F14" s="230" t="s">
         <v>241</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -13694,8 +13849,8 @@
         <f>C21</f>
         <v>200</v>
       </c>
-      <c r="E15" s="215"/>
-      <c r="F15" s="222"/>
+      <c r="E15" s="224"/>
+      <c r="F15" s="231"/>
       <c r="G15" s="145" t="s">
         <v>253</v>
       </c>
@@ -13722,7 +13877,7 @@
         <f>C22</f>
         <v>20</v>
       </c>
-      <c r="E16" s="216"/>
+      <c r="E16" s="225"/>
       <c r="F16" s="79" t="s">
         <v>412</v>
       </c>
@@ -13786,7 +13941,7 @@
         <f>C9*C20</f>
         <v>200</v>
       </c>
-      <c r="E21" s="214" t="s">
+      <c r="E21" s="223" t="s">
         <v>242</v>
       </c>
       <c r="F21" s="71"/>
@@ -13816,7 +13971,7 @@
         <f>C20*10</f>
         <v>20</v>
       </c>
-      <c r="E22" s="215"/>
+      <c r="E22" s="224"/>
       <c r="F22" s="149"/>
       <c r="G22" s="145"/>
       <c r="H22" s="145"/>
@@ -13832,7 +13987,7 @@
         <f>J18/J34</f>
         <v>0.66666666666666674</v>
       </c>
-      <c r="E23" s="216"/>
+      <c r="E23" s="225"/>
       <c r="F23" s="79"/>
       <c r="G23" s="74"/>
       <c r="H23" s="74"/>
@@ -13862,7 +14017,7 @@
     </row>
     <row r="25" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="214" t="s">
+      <c r="E26" s="223" t="s">
         <v>243</v>
       </c>
       <c r="F26" s="71"/>
@@ -13885,7 +14040,7 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="215"/>
+      <c r="E27" s="224"/>
       <c r="F27" s="80"/>
       <c r="G27" s="6" t="s">
         <v>415</v>
@@ -13906,10 +14061,10 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="217" t="s">
+      <c r="B28" s="226" t="s">
         <v>416</v>
       </c>
-      <c r="E28" s="215"/>
+      <c r="E28" s="224"/>
       <c r="F28" s="149"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -13918,8 +14073,8 @@
       <c r="K28" s="150"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="217"/>
-      <c r="E29" s="215"/>
+      <c r="B29" s="226"/>
+      <c r="E29" s="224"/>
       <c r="F29" s="149"/>
       <c r="G29" s="145"/>
       <c r="H29" s="145"/>
@@ -13928,8 +14083,8 @@
       <c r="K29" s="147"/>
     </row>
     <row r="30" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="217"/>
-      <c r="E30" s="216"/>
+      <c r="B30" s="226"/>
+      <c r="E30" s="225"/>
       <c r="F30" s="79"/>
       <c r="G30" s="74" t="s">
         <v>255</v>
@@ -13948,7 +14103,7 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="217"/>
+      <c r="B31" s="226"/>
       <c r="G31" s="82" t="s">
         <v>267</v>
       </c>
@@ -13962,13 +14117,13 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="217"/>
+      <c r="B32" s="226"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="217"/>
+      <c r="B33" s="226"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="217"/>
+      <c r="B34" s="226"/>
       <c r="G34" s="81" t="s">
         <v>264</v>
       </c>
@@ -13986,7 +14141,7 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="217"/>
+      <c r="B35" s="226"/>
     </row>
   </sheetData>
   <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
@@ -14003,12 +14158,12 @@
     <mergeCell ref="F14:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>OR($C$23&lt;60%,$C$23&gt;70%)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>OR($C$24&lt;30%,$C$24&gt;40%)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14041,74 +14196,74 @@
   <sheetData>
     <row r="1" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>375</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="191"/>
+      <c r="O2" s="192"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="184"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="185"/>
-      <c r="L3" s="185"/>
-      <c r="M3" s="185"/>
-      <c r="N3" s="185"/>
-      <c r="O3" s="186"/>
+      <c r="B3" s="193"/>
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="194"/>
+      <c r="H3" s="194"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="194"/>
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="194"/>
+      <c r="O3" s="195"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="196" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="188"/>
-      <c r="D4" s="188"/>
-      <c r="E4" s="188"/>
-      <c r="F4" s="188"/>
-      <c r="G4" s="188"/>
-      <c r="H4" s="188"/>
-      <c r="I4" s="188"/>
-      <c r="J4" s="188"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="188"/>
-      <c r="M4" s="188"/>
-      <c r="N4" s="188"/>
-      <c r="O4" s="189"/>
+      <c r="C4" s="197"/>
+      <c r="D4" s="197"/>
+      <c r="E4" s="197"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
+      <c r="H4" s="197"/>
+      <c r="I4" s="197"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="197"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="197"/>
+      <c r="O4" s="198"/>
     </row>
     <row r="5" spans="2:15" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="199" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="191"/>
-      <c r="D5" s="191"/>
-      <c r="E5" s="191"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="191"/>
-      <c r="H5" s="191"/>
-      <c r="I5" s="191"/>
-      <c r="J5" s="191"/>
-      <c r="K5" s="191"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="191"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="192"/>
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="200"/>
+      <c r="L5" s="200"/>
+      <c r="M5" s="200"/>
+      <c r="N5" s="200"/>
+      <c r="O5" s="201"/>
     </row>
     <row r="6" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -14982,32 +15137,32 @@
     <mergeCell ref="B5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:O7">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>($C$15=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:O16">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>($C$15=2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:O39">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>($C$15=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41:O54">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>OR($C$15=4,$C$15=5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:O56">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>($C$15=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17:O27">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>($C$15=2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15036,32 +15191,32 @@
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="190" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="183"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="223" t="s">
+      <c r="B3" s="232" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
-      <c r="E3" s="224"/>
-      <c r="F3" s="224"/>
-      <c r="G3" s="224"/>
-      <c r="H3" s="224"/>
-      <c r="I3" s="224"/>
-      <c r="J3" s="224"/>
-      <c r="K3" s="225"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">

</xml_diff>

<commit_message>
Added canvas to start our WebGL graphic motor
</commit_message>
<xml_diff>
--- a/documentos/plantilla ABP.xlsx
+++ b/documentos/plantilla ABP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Mixeet\documentos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="500" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
   <definedNames>
     <definedName name="Graficos1">TAG!$F$8:$H$21</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="421">
   <si>
     <t>Apellidos</t>
   </si>
@@ -2097,11 +2102,14 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -3427,6 +3435,15 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3439,16 +3456,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4261,6 +4269,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -4633,8 +4644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4891,7 +4902,9 @@
       <c r="E13" s="60" t="s">
         <v>419</v>
       </c>
-      <c r="F13" s="60"/>
+      <c r="F13" s="60" t="s">
+        <v>420</v>
+      </c>
       <c r="G13" s="60"/>
       <c r="H13" s="60"/>
       <c r="I13" s="60" t="s">
@@ -4899,20 +4912,26 @@
       </c>
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
+      <c r="L13" s="60" t="s">
+        <v>420</v>
+      </c>
       <c r="M13" s="60"/>
       <c r="N13" s="60" t="s">
         <v>419</v>
       </c>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
+      <c r="O13" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="P13" s="61" t="s">
+        <v>420</v>
+      </c>
       <c r="Q13" s="55">
         <f t="shared" ref="Q13:Q18" si="0">COUNTIF(E13:P13,"*")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R13" s="56">
         <f>Q13*10</f>
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -5065,7 +5084,7 @@
       </c>
       <c r="F19" s="57">
         <f t="shared" ref="F19:P19" si="2">COUNTIF(F13:F18,"*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="57">
         <f t="shared" si="2"/>
@@ -5089,7 +5108,7 @@
       </c>
       <c r="L19" s="57">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="57">
         <f t="shared" si="2"/>
@@ -5101,15 +5120,15 @@
       </c>
       <c r="O19" s="57">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="57">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="56">
         <f>SUM(Q13:Q18)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="R19" s="56"/>
     </row>
@@ -5125,7 +5144,7 @@
       </c>
       <c r="F20" s="56">
         <f t="shared" ref="F20:P20" si="3">F19*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G20" s="56">
         <f t="shared" si="3"/>
@@ -5149,7 +5168,7 @@
       </c>
       <c r="L20" s="56">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M20" s="56">
         <f t="shared" si="3"/>
@@ -5161,15 +5180,15 @@
       </c>
       <c r="O20" s="56">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P20" s="56">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R20" s="56">
         <f>SUM(R13:R18)</f>
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
@@ -5442,8 +5461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5653,18 +5672,20 @@
       <c r="F11" s="128">
         <v>2</v>
       </c>
-      <c r="G11" s="155"/>
+      <c r="G11" s="155">
+        <v>2</v>
+      </c>
       <c r="H11" s="129">
         <v>0.1</v>
       </c>
       <c r="I11" s="128">
         <f>$C$17*H11</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J11" s="155"/>
       <c r="K11" s="128">
         <f>$C$20*H11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="157"/>
       <c r="M11" s="5"/>
@@ -5686,18 +5707,20 @@
       <c r="F12" s="128">
         <v>2</v>
       </c>
-      <c r="G12" s="155"/>
+      <c r="G12" s="155">
+        <v>2</v>
+      </c>
       <c r="H12" s="129">
         <v>0.25</v>
       </c>
       <c r="I12" s="128">
         <f t="shared" ref="I12:I15" si="0">$C$17*H12</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J12" s="155"/>
       <c r="K12" s="128">
         <f t="shared" ref="K12:K15" si="1">$C$20*H12</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L12" s="157"/>
       <c r="M12" s="5"/>
@@ -5718,12 +5741,12 @@
       </c>
       <c r="I13" s="128">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="J13" s="155"/>
       <c r="K13" s="128">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L13" s="157"/>
       <c r="M13" s="5"/>
@@ -5744,12 +5767,12 @@
       </c>
       <c r="I14" s="128">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J14" s="155"/>
       <c r="K14" s="128">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="157"/>
       <c r="M14" s="5"/>
@@ -5773,12 +5796,12 @@
       </c>
       <c r="I15" s="128">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J15" s="156"/>
       <c r="K15" s="128">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="158"/>
       <c r="M15" s="5"/>
@@ -5792,7 +5815,7 @@
       </c>
       <c r="C16" s="6">
         <f>'Principal - ABP'!O19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -5805,7 +5828,7 @@
       </c>
       <c r="C17" s="6">
         <f>C10*C16</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E17" s="140" t="s">
         <v>146</v>
@@ -5818,7 +5841,7 @@
       </c>
       <c r="I17" s="143">
         <f t="shared" ref="I17:L17" si="2">SUM(I11:I15)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J17" s="143">
         <f t="shared" si="2"/>
@@ -5826,7 +5849,7 @@
       </c>
       <c r="K17" s="143">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L17" s="144">
         <f t="shared" si="2"/>
@@ -5859,9 +5882,9 @@
       <c r="B19" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="11" t="str">
+      <c r="C19" s="11">
         <f>IF(C17=0,"-",C18/C17-1)</f>
-        <v>-</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -5870,7 +5893,7 @@
       </c>
       <c r="C20" s="6">
         <f>C16*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -6003,7 +6026,7 @@
       </c>
       <c r="C13" s="6">
         <f>'Principal - ABP'!P19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -6012,7 +6035,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6034,7 +6057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -7750,7 +7773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
@@ -7845,7 +7868,7 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="207" t="s">
+      <c r="E8" s="210" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -7863,7 +7886,7 @@
       <c r="J8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="210" t="s">
+      <c r="K8" s="213" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7874,7 +7897,7 @@
       <c r="C9" s="6">
         <v>120</v>
       </c>
-      <c r="E9" s="208"/>
+      <c r="E9" s="211"/>
       <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
@@ -7890,7 +7913,7 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="211"/>
+      <c r="K9" s="208"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
@@ -7899,7 +7922,7 @@
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="208"/>
+      <c r="E10" s="211"/>
       <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
@@ -7915,7 +7938,7 @@
       <c r="J10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="212"/>
+      <c r="K10" s="214"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -7925,7 +7948,7 @@
         <f>SUM(C8:C10)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="208"/>
+      <c r="E11" s="211"/>
       <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
@@ -7941,12 +7964,12 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="213" t="s">
+      <c r="K11" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="208"/>
+      <c r="E12" s="211"/>
       <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
@@ -7962,10 +7985,10 @@
       <c r="J12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="211"/>
+      <c r="K12" s="208"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="208"/>
+      <c r="E13" s="211"/>
       <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
@@ -7981,13 +8004,13 @@
       <c r="J13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K13" s="211"/>
+      <c r="K13" s="208"/>
     </row>
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="208"/>
+      <c r="E14" s="211"/>
       <c r="F14" s="2" t="s">
         <v>62</v>
       </c>
@@ -8003,7 +8026,7 @@
       <c r="J14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="211"/>
+      <c r="K14" s="208"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -8011,9 +8034,9 @@
       </c>
       <c r="C15" s="6">
         <f>'Principal - ABP'!F19</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="208"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="211"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -8029,7 +8052,7 @@
       <c r="J15" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="211"/>
+      <c r="K15" s="208"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -8037,9 +8060,9 @@
       </c>
       <c r="C16" s="6">
         <f>C9*C15</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="208"/>
+        <v>120</v>
+      </c>
+      <c r="E16" s="211"/>
       <c r="F16" s="2" t="s">
         <v>64</v>
       </c>
@@ -8055,7 +8078,7 @@
       <c r="J16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="212"/>
+      <c r="K16" s="214"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -8063,9 +8086,9 @@
       </c>
       <c r="C17" s="6">
         <f>(IF(C15=1,H21,IF(C15=2,H37,IF(C15=3,H55,IF(C15=4,H76,IF(C15=5,H97,H118))))))</f>
-        <v>574</v>
-      </c>
-      <c r="E17" s="208"/>
+        <v>101</v>
+      </c>
+      <c r="E17" s="211"/>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
@@ -8081,7 +8104,7 @@
       <c r="J17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="213" t="s">
+      <c r="K17" s="207" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8089,11 +8112,11 @@
       <c r="B18" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="11" t="e">
+      <c r="C18" s="11">
         <f>C17/C16-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="208"/>
+        <v>-0.15833333333333333</v>
+      </c>
+      <c r="E18" s="211"/>
       <c r="F18" s="2" t="s">
         <v>66</v>
       </c>
@@ -8109,7 +8132,7 @@
       <c r="J18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K18" s="211"/>
+      <c r="K18" s="208"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -8117,9 +8140,9 @@
       </c>
       <c r="C19" s="6">
         <f>C15*10</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="208"/>
+        <v>10</v>
+      </c>
+      <c r="E19" s="211"/>
       <c r="F19" s="2" t="s">
         <v>67</v>
       </c>
@@ -8135,7 +8158,7 @@
       <c r="J19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="211"/>
+      <c r="K19" s="208"/>
     </row>
     <row r="20" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
@@ -8143,9 +8166,9 @@
       </c>
       <c r="C20" s="6">
         <f>IF(C15=1,I21,IF(C15=2,I37,IF(C15=3,I55,IF(C15=4,I76,IF(C15=5,I97,I118)))))</f>
-        <v>60.000000000000007</v>
-      </c>
-      <c r="E20" s="209"/>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="E20" s="212"/>
       <c r="F20" s="4" t="s">
         <v>68</v>
       </c>
@@ -8161,7 +8184,7 @@
       <c r="J20" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="214"/>
+      <c r="K20" s="209"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
@@ -8188,7 +8211,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="207" t="s">
+      <c r="E23" s="210" t="s">
         <v>141</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -8206,12 +8229,12 @@
       <c r="J23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="210" t="s">
+      <c r="K23" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="208"/>
+      <c r="E24" s="211"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
@@ -8227,10 +8250,10 @@
       <c r="J24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="211"/>
+      <c r="K24" s="208"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="208"/>
+      <c r="E25" s="211"/>
       <c r="F25" s="2" t="s">
         <v>58</v>
       </c>
@@ -8246,10 +8269,10 @@
       <c r="J25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K25" s="212"/>
+      <c r="K25" s="214"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="208"/>
+      <c r="E26" s="211"/>
       <c r="F26" s="2" t="s">
         <v>59</v>
       </c>
@@ -8265,12 +8288,12 @@
       <c r="J26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="213" t="s">
+      <c r="K26" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="208"/>
+      <c r="E27" s="211"/>
       <c r="F27" s="2" t="s">
         <v>60</v>
       </c>
@@ -8286,10 +8309,10 @@
       <c r="J27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="211"/>
+      <c r="K27" s="208"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="208"/>
+      <c r="E28" s="211"/>
       <c r="F28" s="2" t="s">
         <v>61</v>
       </c>
@@ -8305,10 +8328,10 @@
       <c r="J28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="211"/>
+      <c r="K28" s="208"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="208"/>
+      <c r="E29" s="211"/>
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
@@ -8324,10 +8347,10 @@
       <c r="J29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="211"/>
+      <c r="K29" s="208"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="208"/>
+      <c r="E30" s="211"/>
       <c r="F30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8343,10 +8366,10 @@
       <c r="J30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="211"/>
+      <c r="K30" s="208"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="208"/>
+      <c r="E31" s="211"/>
       <c r="F31" s="2" t="s">
         <v>64</v>
       </c>
@@ -8362,10 +8385,10 @@
       <c r="J31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K31" s="211"/>
+      <c r="K31" s="208"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="208"/>
+      <c r="E32" s="211"/>
       <c r="F32" s="2" t="s">
         <v>65</v>
       </c>
@@ -8381,10 +8404,10 @@
       <c r="J32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="212"/>
+      <c r="K32" s="214"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E33" s="208"/>
+      <c r="E33" s="211"/>
       <c r="F33" s="2" t="s">
         <v>66</v>
       </c>
@@ -8400,12 +8423,12 @@
       <c r="J33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K33" s="213" t="s">
+      <c r="K33" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" s="208"/>
+      <c r="E34" s="211"/>
       <c r="F34" s="2" t="s">
         <v>67</v>
       </c>
@@ -8421,10 +8444,10 @@
       <c r="J34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K34" s="211"/>
+      <c r="K34" s="208"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E35" s="208"/>
+      <c r="E35" s="211"/>
       <c r="F35" s="2" t="s">
         <v>68</v>
       </c>
@@ -8440,10 +8463,10 @@
       <c r="J35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K35" s="211"/>
+      <c r="K35" s="208"/>
     </row>
     <row r="36" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="209"/>
+      <c r="E36" s="212"/>
       <c r="F36" s="4" t="s">
         <v>69</v>
       </c>
@@ -8459,7 +8482,7 @@
       <c r="J36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K36" s="214"/>
+      <c r="K36" s="209"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
@@ -8486,7 +8509,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E39" s="207" t="s">
+      <c r="E39" s="210" t="s">
         <v>142</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -8504,12 +8527,12 @@
       <c r="J39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K39" s="210" t="s">
+      <c r="K39" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E40" s="208"/>
+      <c r="E40" s="211"/>
       <c r="F40" s="2" t="s">
         <v>57</v>
       </c>
@@ -8525,10 +8548,10 @@
       <c r="J40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K40" s="211"/>
+      <c r="K40" s="208"/>
     </row>
     <row r="41" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E41" s="208"/>
+      <c r="E41" s="211"/>
       <c r="F41" s="2" t="s">
         <v>58</v>
       </c>
@@ -8544,10 +8567,10 @@
       <c r="J41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K41" s="212"/>
+      <c r="K41" s="214"/>
     </row>
     <row r="42" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E42" s="208"/>
+      <c r="E42" s="211"/>
       <c r="F42" s="2" t="s">
         <v>59</v>
       </c>
@@ -8563,12 +8586,12 @@
       <c r="J42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K42" s="213" t="s">
+      <c r="K42" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E43" s="208"/>
+      <c r="E43" s="211"/>
       <c r="F43" s="2" t="s">
         <v>60</v>
       </c>
@@ -8584,10 +8607,10 @@
       <c r="J43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K43" s="211"/>
+      <c r="K43" s="208"/>
     </row>
     <row r="44" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E44" s="208"/>
+      <c r="E44" s="211"/>
       <c r="F44" s="2" t="s">
         <v>61</v>
       </c>
@@ -8603,10 +8626,10 @@
       <c r="J44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K44" s="211"/>
+      <c r="K44" s="208"/>
     </row>
     <row r="45" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E45" s="208"/>
+      <c r="E45" s="211"/>
       <c r="F45" s="2" t="s">
         <v>62</v>
       </c>
@@ -8622,10 +8645,10 @@
       <c r="J45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K45" s="211"/>
+      <c r="K45" s="208"/>
     </row>
     <row r="46" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E46" s="208"/>
+      <c r="E46" s="211"/>
       <c r="F46" s="2" t="s">
         <v>63</v>
       </c>
@@ -8641,10 +8664,10 @@
       <c r="J46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K46" s="211"/>
+      <c r="K46" s="208"/>
     </row>
     <row r="47" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E47" s="208"/>
+      <c r="E47" s="211"/>
       <c r="F47" s="2" t="s">
         <v>64</v>
       </c>
@@ -8660,10 +8683,10 @@
       <c r="J47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K47" s="211"/>
+      <c r="K47" s="208"/>
     </row>
     <row r="48" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E48" s="208"/>
+      <c r="E48" s="211"/>
       <c r="F48" s="2" t="s">
         <v>65</v>
       </c>
@@ -8679,10 +8702,10 @@
       <c r="J48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K48" s="211"/>
+      <c r="K48" s="208"/>
     </row>
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E49" s="208"/>
+      <c r="E49" s="211"/>
       <c r="F49" s="2" t="s">
         <v>66</v>
       </c>
@@ -8698,10 +8721,10 @@
       <c r="J49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K49" s="211"/>
+      <c r="K49" s="208"/>
     </row>
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E50" s="208"/>
+      <c r="E50" s="211"/>
       <c r="F50" s="2" t="s">
         <v>67</v>
       </c>
@@ -8717,10 +8740,10 @@
       <c r="J50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K50" s="212"/>
+      <c r="K50" s="214"/>
     </row>
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E51" s="208"/>
+      <c r="E51" s="211"/>
       <c r="F51" s="2" t="s">
         <v>68</v>
       </c>
@@ -8736,12 +8759,12 @@
       <c r="J51" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K51" s="213" t="s">
+      <c r="K51" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E52" s="208"/>
+      <c r="E52" s="211"/>
       <c r="F52" s="2" t="s">
         <v>69</v>
       </c>
@@ -8757,10 +8780,10 @@
       <c r="J52" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K52" s="211"/>
+      <c r="K52" s="208"/>
     </row>
     <row r="53" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E53" s="208"/>
+      <c r="E53" s="211"/>
       <c r="F53" s="2" t="s">
         <v>70</v>
       </c>
@@ -8776,10 +8799,10 @@
       <c r="J53" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K53" s="211"/>
+      <c r="K53" s="208"/>
     </row>
     <row r="54" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="209"/>
+      <c r="E54" s="212"/>
       <c r="F54" s="4" t="s">
         <v>71</v>
       </c>
@@ -8795,7 +8818,7 @@
       <c r="J54" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K54" s="214"/>
+      <c r="K54" s="209"/>
     </row>
     <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
@@ -8822,7 +8845,7 @@
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E57" s="207" t="s">
+      <c r="E57" s="210" t="s">
         <v>143</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -8840,12 +8863,12 @@
       <c r="J57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K57" s="210" t="s">
+      <c r="K57" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E58" s="208"/>
+      <c r="E58" s="211"/>
       <c r="F58" s="2" t="s">
         <v>57</v>
       </c>
@@ -8861,10 +8884,10 @@
       <c r="J58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K58" s="211"/>
+      <c r="K58" s="208"/>
     </row>
     <row r="59" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E59" s="208"/>
+      <c r="E59" s="211"/>
       <c r="F59" s="2" t="s">
         <v>58</v>
       </c>
@@ -8880,10 +8903,10 @@
       <c r="J59" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K59" s="212"/>
+      <c r="K59" s="214"/>
     </row>
     <row r="60" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E60" s="208"/>
+      <c r="E60" s="211"/>
       <c r="F60" s="2" t="s">
         <v>59</v>
       </c>
@@ -8899,12 +8922,12 @@
       <c r="J60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K60" s="213" t="s">
+      <c r="K60" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E61" s="208"/>
+      <c r="E61" s="211"/>
       <c r="F61" s="2" t="s">
         <v>60</v>
       </c>
@@ -8920,10 +8943,10 @@
       <c r="J61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K61" s="211"/>
+      <c r="K61" s="208"/>
     </row>
     <row r="62" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E62" s="208"/>
+      <c r="E62" s="211"/>
       <c r="F62" s="2" t="s">
         <v>61</v>
       </c>
@@ -8939,10 +8962,10 @@
       <c r="J62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K62" s="211"/>
+      <c r="K62" s="208"/>
     </row>
     <row r="63" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E63" s="208"/>
+      <c r="E63" s="211"/>
       <c r="F63" s="2" t="s">
         <v>62</v>
       </c>
@@ -8958,10 +8981,10 @@
       <c r="J63" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K63" s="211"/>
+      <c r="K63" s="208"/>
     </row>
     <row r="64" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="208"/>
+      <c r="E64" s="211"/>
       <c r="F64" s="2" t="s">
         <v>63</v>
       </c>
@@ -8977,10 +9000,10 @@
       <c r="J64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K64" s="211"/>
+      <c r="K64" s="208"/>
     </row>
     <row r="65" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E65" s="208"/>
+      <c r="E65" s="211"/>
       <c r="F65" s="2" t="s">
         <v>64</v>
       </c>
@@ -8996,10 +9019,10 @@
       <c r="J65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K65" s="211"/>
+      <c r="K65" s="208"/>
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E66" s="208"/>
+      <c r="E66" s="211"/>
       <c r="F66" s="2" t="s">
         <v>65</v>
       </c>
@@ -9015,10 +9038,10 @@
       <c r="J66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K66" s="211"/>
+      <c r="K66" s="208"/>
     </row>
     <row r="67" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E67" s="208"/>
+      <c r="E67" s="211"/>
       <c r="F67" s="2" t="s">
         <v>66</v>
       </c>
@@ -9034,10 +9057,10 @@
       <c r="J67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K67" s="211"/>
+      <c r="K67" s="208"/>
     </row>
     <row r="68" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E68" s="208"/>
+      <c r="E68" s="211"/>
       <c r="F68" s="2" t="s">
         <v>67</v>
       </c>
@@ -9053,10 +9076,10 @@
       <c r="J68" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K68" s="211"/>
+      <c r="K68" s="208"/>
     </row>
     <row r="69" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E69" s="208"/>
+      <c r="E69" s="211"/>
       <c r="F69" s="2" t="s">
         <v>68</v>
       </c>
@@ -9072,10 +9095,10 @@
       <c r="J69" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K69" s="211"/>
+      <c r="K69" s="208"/>
     </row>
     <row r="70" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E70" s="208"/>
+      <c r="E70" s="211"/>
       <c r="F70" s="2" t="s">
         <v>69</v>
       </c>
@@ -9091,10 +9114,10 @@
       <c r="J70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K70" s="211"/>
+      <c r="K70" s="208"/>
     </row>
     <row r="71" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E71" s="208"/>
+      <c r="E71" s="211"/>
       <c r="F71" s="2" t="s">
         <v>70</v>
       </c>
@@ -9110,10 +9133,10 @@
       <c r="J71" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K71" s="212"/>
+      <c r="K71" s="214"/>
     </row>
     <row r="72" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E72" s="208"/>
+      <c r="E72" s="211"/>
       <c r="F72" s="2" t="s">
         <v>71</v>
       </c>
@@ -9129,12 +9152,12 @@
       <c r="J72" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K72" s="213" t="s">
+      <c r="K72" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E73" s="208"/>
+      <c r="E73" s="211"/>
       <c r="F73" s="2" t="s">
         <v>72</v>
       </c>
@@ -9150,10 +9173,10 @@
       <c r="J73" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K73" s="211"/>
+      <c r="K73" s="208"/>
     </row>
     <row r="74" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E74" s="208"/>
+      <c r="E74" s="211"/>
       <c r="F74" s="2" t="s">
         <v>73</v>
       </c>
@@ -9169,10 +9192,10 @@
       <c r="J74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K74" s="211"/>
+      <c r="K74" s="208"/>
     </row>
     <row r="75" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E75" s="209"/>
+      <c r="E75" s="212"/>
       <c r="F75" s="4" t="s">
         <v>74</v>
       </c>
@@ -9188,7 +9211,7 @@
       <c r="J75" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K75" s="214"/>
+      <c r="K75" s="209"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
@@ -9208,7 +9231,7 @@
     </row>
     <row r="77" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E78" s="207" t="s">
+      <c r="E78" s="210" t="s">
         <v>144</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -9231,7 +9254,7 @@
       </c>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E79" s="208"/>
+      <c r="E79" s="211"/>
       <c r="F79" s="2" t="s">
         <v>57</v>
       </c>
@@ -9250,7 +9273,7 @@
       <c r="K79" s="216"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E80" s="208"/>
+      <c r="E80" s="211"/>
       <c r="F80" s="2" t="s">
         <v>58</v>
       </c>
@@ -9269,7 +9292,7 @@
       <c r="K80" s="217"/>
     </row>
     <row r="81" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E81" s="208"/>
+      <c r="E81" s="211"/>
       <c r="F81" s="2" t="s">
         <v>59</v>
       </c>
@@ -9285,12 +9308,12 @@
       <c r="J81" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K81" s="213" t="s">
+      <c r="K81" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E82" s="208"/>
+      <c r="E82" s="211"/>
       <c r="F82" s="2" t="s">
         <v>60</v>
       </c>
@@ -9306,10 +9329,10 @@
       <c r="J82" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K82" s="211"/>
+      <c r="K82" s="208"/>
     </row>
     <row r="83" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E83" s="208"/>
+      <c r="E83" s="211"/>
       <c r="F83" s="2" t="s">
         <v>61</v>
       </c>
@@ -9325,10 +9348,10 @@
       <c r="J83" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K83" s="211"/>
+      <c r="K83" s="208"/>
     </row>
     <row r="84" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E84" s="208"/>
+      <c r="E84" s="211"/>
       <c r="F84" s="2" t="s">
         <v>62</v>
       </c>
@@ -9344,10 +9367,10 @@
       <c r="J84" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K84" s="211"/>
+      <c r="K84" s="208"/>
     </row>
     <row r="85" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E85" s="208"/>
+      <c r="E85" s="211"/>
       <c r="F85" s="2" t="s">
         <v>63</v>
       </c>
@@ -9363,10 +9386,10 @@
       <c r="J85" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K85" s="211"/>
+      <c r="K85" s="208"/>
     </row>
     <row r="86" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E86" s="208"/>
+      <c r="E86" s="211"/>
       <c r="F86" s="2" t="s">
         <v>64</v>
       </c>
@@ -9382,10 +9405,10 @@
       <c r="J86" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K86" s="211"/>
+      <c r="K86" s="208"/>
     </row>
     <row r="87" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E87" s="208"/>
+      <c r="E87" s="211"/>
       <c r="F87" s="2" t="s">
         <v>65</v>
       </c>
@@ -9401,10 +9424,10 @@
       <c r="J87" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K87" s="211"/>
+      <c r="K87" s="208"/>
     </row>
     <row r="88" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E88" s="208"/>
+      <c r="E88" s="211"/>
       <c r="F88" s="2" t="s">
         <v>66</v>
       </c>
@@ -9420,10 +9443,10 @@
       <c r="J88" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K88" s="211"/>
+      <c r="K88" s="208"/>
     </row>
     <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="208"/>
+      <c r="E89" s="211"/>
       <c r="F89" s="2" t="s">
         <v>67</v>
       </c>
@@ -9439,10 +9462,10 @@
       <c r="J89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K89" s="211"/>
+      <c r="K89" s="208"/>
     </row>
     <row r="90" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E90" s="208"/>
+      <c r="E90" s="211"/>
       <c r="F90" s="2" t="s">
         <v>68</v>
       </c>
@@ -9458,10 +9481,10 @@
       <c r="J90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K90" s="211"/>
+      <c r="K90" s="208"/>
     </row>
     <row r="91" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E91" s="208"/>
+      <c r="E91" s="211"/>
       <c r="F91" s="2" t="s">
         <v>69</v>
       </c>
@@ -9477,10 +9500,10 @@
       <c r="J91" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K91" s="211"/>
+      <c r="K91" s="208"/>
     </row>
     <row r="92" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E92" s="208"/>
+      <c r="E92" s="211"/>
       <c r="F92" s="2" t="s">
         <v>70</v>
       </c>
@@ -9496,10 +9519,10 @@
       <c r="J92" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K92" s="211"/>
+      <c r="K92" s="208"/>
     </row>
     <row r="93" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E93" s="208"/>
+      <c r="E93" s="211"/>
       <c r="F93" s="2" t="s">
         <v>71</v>
       </c>
@@ -9515,10 +9538,10 @@
       <c r="J93" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K93" s="212"/>
+      <c r="K93" s="214"/>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E94" s="208"/>
+      <c r="E94" s="211"/>
       <c r="F94" s="2" t="s">
         <v>72</v>
       </c>
@@ -9534,12 +9557,12 @@
       <c r="J94" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K94" s="213" t="s">
+      <c r="K94" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E95" s="208"/>
+      <c r="E95" s="211"/>
       <c r="F95" s="2" t="s">
         <v>73</v>
       </c>
@@ -9555,10 +9578,10 @@
       <c r="J95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K95" s="211"/>
+      <c r="K95" s="208"/>
     </row>
     <row r="96" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E96" s="209"/>
+      <c r="E96" s="212"/>
       <c r="F96" s="4" t="s">
         <v>74</v>
       </c>
@@ -9574,7 +9597,7 @@
       <c r="J96" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K96" s="214"/>
+      <c r="K96" s="209"/>
     </row>
     <row r="97" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
@@ -9594,7 +9617,7 @@
     </row>
     <row r="98" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E99" s="207" t="s">
+      <c r="E99" s="210" t="s">
         <v>145</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -9612,12 +9635,12 @@
       <c r="J99" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K99" s="210" t="s">
+      <c r="K99" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="100" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E100" s="208"/>
+      <c r="E100" s="211"/>
       <c r="F100" s="2" t="s">
         <v>57</v>
       </c>
@@ -9633,10 +9656,10 @@
       <c r="J100" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K100" s="211"/>
+      <c r="K100" s="208"/>
     </row>
     <row r="101" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E101" s="208"/>
+      <c r="E101" s="211"/>
       <c r="F101" s="2" t="s">
         <v>58</v>
       </c>
@@ -9652,10 +9675,10 @@
       <c r="J101" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K101" s="212"/>
+      <c r="K101" s="214"/>
     </row>
     <row r="102" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E102" s="208"/>
+      <c r="E102" s="211"/>
       <c r="F102" s="2" t="s">
         <v>59</v>
       </c>
@@ -9671,12 +9694,12 @@
       <c r="J102" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K102" s="213" t="s">
+      <c r="K102" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="103" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E103" s="208"/>
+      <c r="E103" s="211"/>
       <c r="F103" s="2" t="s">
         <v>60</v>
       </c>
@@ -9692,10 +9715,10 @@
       <c r="J103" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K103" s="211"/>
+      <c r="K103" s="208"/>
     </row>
     <row r="104" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E104" s="208"/>
+      <c r="E104" s="211"/>
       <c r="F104" s="2" t="s">
         <v>61</v>
       </c>
@@ -9711,10 +9734,10 @@
       <c r="J104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K104" s="211"/>
+      <c r="K104" s="208"/>
     </row>
     <row r="105" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E105" s="208"/>
+      <c r="E105" s="211"/>
       <c r="F105" s="2" t="s">
         <v>62</v>
       </c>
@@ -9730,10 +9753,10 @@
       <c r="J105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K105" s="211"/>
+      <c r="K105" s="208"/>
     </row>
     <row r="106" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E106" s="208"/>
+      <c r="E106" s="211"/>
       <c r="F106" s="2" t="s">
         <v>63</v>
       </c>
@@ -9749,10 +9772,10 @@
       <c r="J106" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K106" s="211"/>
+      <c r="K106" s="208"/>
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E107" s="208"/>
+      <c r="E107" s="211"/>
       <c r="F107" s="2" t="s">
         <v>64</v>
       </c>
@@ -9768,10 +9791,10 @@
       <c r="J107" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K107" s="211"/>
+      <c r="K107" s="208"/>
     </row>
     <row r="108" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E108" s="208"/>
+      <c r="E108" s="211"/>
       <c r="F108" s="2" t="s">
         <v>65</v>
       </c>
@@ -9787,10 +9810,10 @@
       <c r="J108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K108" s="211"/>
+      <c r="K108" s="208"/>
     </row>
     <row r="109" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E109" s="208"/>
+      <c r="E109" s="211"/>
       <c r="F109" s="2" t="s">
         <v>66</v>
       </c>
@@ -9806,10 +9829,10 @@
       <c r="J109" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K109" s="211"/>
+      <c r="K109" s="208"/>
     </row>
     <row r="110" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E110" s="208"/>
+      <c r="E110" s="211"/>
       <c r="F110" s="2" t="s">
         <v>67</v>
       </c>
@@ -9825,10 +9848,10 @@
       <c r="J110" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K110" s="211"/>
+      <c r="K110" s="208"/>
     </row>
     <row r="111" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E111" s="208"/>
+      <c r="E111" s="211"/>
       <c r="F111" s="2" t="s">
         <v>68</v>
       </c>
@@ -9844,10 +9867,10 @@
       <c r="J111" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K111" s="211"/>
+      <c r="K111" s="208"/>
     </row>
     <row r="112" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E112" s="208"/>
+      <c r="E112" s="211"/>
       <c r="F112" s="2" t="s">
         <v>69</v>
       </c>
@@ -9863,10 +9886,10 @@
       <c r="J112" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K112" s="211"/>
+      <c r="K112" s="208"/>
     </row>
     <row r="113" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E113" s="208"/>
+      <c r="E113" s="211"/>
       <c r="F113" s="2" t="s">
         <v>70</v>
       </c>
@@ -9882,10 +9905,10 @@
       <c r="J113" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K113" s="211"/>
+      <c r="K113" s="208"/>
     </row>
     <row r="114" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E114" s="208"/>
+      <c r="E114" s="211"/>
       <c r="F114" s="2" t="s">
         <v>71</v>
       </c>
@@ -9901,10 +9924,10 @@
       <c r="J114" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K114" s="211"/>
+      <c r="K114" s="208"/>
     </row>
     <row r="115" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E115" s="208"/>
+      <c r="E115" s="211"/>
       <c r="F115" s="2" t="s">
         <v>72</v>
       </c>
@@ -9920,10 +9943,10 @@
       <c r="J115" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K115" s="212"/>
+      <c r="K115" s="214"/>
     </row>
     <row r="116" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E116" s="208"/>
+      <c r="E116" s="211"/>
       <c r="F116" s="2" t="s">
         <v>73</v>
       </c>
@@ -9939,12 +9962,12 @@
       <c r="J116" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K116" s="213" t="s">
+      <c r="K116" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="209"/>
+      <c r="E117" s="212"/>
       <c r="F117" s="4" t="s">
         <v>74</v>
       </c>
@@ -9960,7 +9983,7 @@
       <c r="J117" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K117" s="214"/>
+      <c r="K117" s="209"/>
     </row>
     <row r="118" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F118" s="1"/>
@@ -9981,18 +10004,6 @@
   </sheetData>
   <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="E8:E20"/>
-    <mergeCell ref="E23:E36"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K16"/>
-    <mergeCell ref="K17:K20"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="K26:K32"/>
     <mergeCell ref="E99:E117"/>
     <mergeCell ref="K99:K101"/>
     <mergeCell ref="K102:K115"/>
@@ -10009,6 +10020,18 @@
     <mergeCell ref="E39:E54"/>
     <mergeCell ref="E57:E75"/>
     <mergeCell ref="E78:E96"/>
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="E8:E20"/>
+    <mergeCell ref="E23:E36"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K26:K32"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:K21">
     <cfRule type="expression" dxfId="63" priority="7">
@@ -15267,7 +15290,7 @@
       </c>
       <c r="C13" s="6">
         <f>'Principal - ABP'!L19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -15276,7 +15299,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last changes + ITERACIONES HITO 2
</commit_message>
<xml_diff>
--- a/documentos/plantilla ABP.xlsx
+++ b/documentos/plantilla ABP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="500" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="500" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,24 @@
     <sheet name="V1" sheetId="6" r:id="rId4"/>
     <sheet name="V2" sheetId="7" r:id="rId5"/>
     <sheet name="PD" sheetId="2" r:id="rId6"/>
-    <sheet name="TDS" sheetId="10" r:id="rId7"/>
-    <sheet name="RV" sheetId="11" r:id="rId8"/>
-    <sheet name="SMBI" sheetId="8" r:id="rId9"/>
-    <sheet name="EL" sheetId="12" r:id="rId10"/>
-    <sheet name="SDM" sheetId="13" r:id="rId11"/>
-    <sheet name="SMA" sheetId="14" r:id="rId12"/>
-    <sheet name="NM" sheetId="15" r:id="rId13"/>
+    <sheet name="Hoja1" sheetId="18" r:id="rId7"/>
+    <sheet name="TDS" sheetId="10" r:id="rId8"/>
+    <sheet name="RV" sheetId="11" r:id="rId9"/>
+    <sheet name="SMBI" sheetId="8" r:id="rId10"/>
+    <sheet name="EL" sheetId="12" r:id="rId11"/>
+    <sheet name="SDM" sheetId="13" r:id="rId12"/>
+    <sheet name="SMA" sheetId="14" r:id="rId13"/>
     <sheet name="PD1" sheetId="17" r:id="rId14"/>
+    <sheet name="NM" sheetId="15" r:id="rId15"/>
+    <sheet name="Hoja2" sheetId="19" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId17"/>
   </externalReferences>
   <definedNames>
     <definedName name="Graficos1">TAG!$F$8:$H$21</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3435,6 +3437,15 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3447,16 +3458,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5231,13 +5233,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="190" t="s">
-        <v>364</v>
+        <v>234</v>
       </c>
       <c r="C2" s="191"/>
       <c r="D2" s="191"/>
@@ -5265,7 +5267,7 @@
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>365</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -5303,7 +5305,7 @@
     </row>
     <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>366</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -5311,8 +5313,8 @@
         <v>110</v>
       </c>
       <c r="C13" s="6">
-        <f>'Principal - ABP'!M19</f>
-        <v>0</v>
+        <f>'Principal - ABP'!L19</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -5321,7 +5323,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5331,6 +5333,7 @@
     <mergeCell ref="B3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5355,7 +5358,7 @@
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="190" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C2" s="191"/>
       <c r="D2" s="191"/>
@@ -5383,7 +5386,7 @@
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -5421,7 +5424,7 @@
     </row>
     <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -5429,8 +5432,8 @@
         <v>110</v>
       </c>
       <c r="C13" s="6">
-        <f>'Principal - ABP'!N19</f>
-        <v>1</v>
+        <f>'Principal - ABP'!M19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -5439,7 +5442,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5459,9 +5462,127 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="190" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
+    </row>
+    <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="232" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
+    </row>
+    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="6">
+        <f>SUM(C6:C8)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="25" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="6">
+        <f>'Principal - ABP'!N19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="6">
+        <f>C13*10</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -5941,7 +6062,139 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="161"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="162"/>
+      <c r="B2" s="163"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="164"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="162" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="163" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="163" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="164" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="163"/>
+      <c r="C4" s="162" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="163" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="163"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
+      <c r="K4" s="167">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="163" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="163"/>
+      <c r="C5" s="165" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="163" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
+      <c r="K5" s="167">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="165"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="165" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="165"/>
+      <c r="I6" s="165"/>
+      <c r="J6" s="165"/>
+      <c r="K6" s="166">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:K3 B4:K4 A5:K6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>($C$15=1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K14"/>
   <sheetViews>
@@ -6059,136 +6312,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="161"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="162"/>
-      <c r="B2" s="163"/>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="164"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="162" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="163" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="163" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="163"/>
-      <c r="K3" s="164" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="162" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="163" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="167">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="163" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="163" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="167">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="165" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="165"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="165"/>
-      <c r="F6" s="165" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="165" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="165"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="165"/>
-      <c r="K6" s="166">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:K6">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>($C$15=1)</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6196,8 +6328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7779,8 +7911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7874,7 +8006,7 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="207" t="s">
+      <c r="E8" s="210" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -7892,7 +8024,7 @@
       <c r="J8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="210" t="s">
+      <c r="K8" s="213" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7903,7 +8035,7 @@
       <c r="C9" s="6">
         <v>120</v>
       </c>
-      <c r="E9" s="208"/>
+      <c r="E9" s="211"/>
       <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
@@ -7919,7 +8051,7 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="211"/>
+      <c r="K9" s="208"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
@@ -7928,7 +8060,7 @@
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="208"/>
+      <c r="E10" s="211"/>
       <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
@@ -7944,7 +8076,7 @@
       <c r="J10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="212"/>
+      <c r="K10" s="214"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -7954,7 +8086,7 @@
         <f>SUM(C8:C10)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="208"/>
+      <c r="E11" s="211"/>
       <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
@@ -7970,12 +8102,12 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="213" t="s">
+      <c r="K11" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="208"/>
+      <c r="E12" s="211"/>
       <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
@@ -7991,10 +8123,10 @@
       <c r="J12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="211"/>
+      <c r="K12" s="208"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="208"/>
+      <c r="E13" s="211"/>
       <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
@@ -8010,13 +8142,13 @@
       <c r="J13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K13" s="211"/>
+      <c r="K13" s="208"/>
     </row>
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="208"/>
+      <c r="E14" s="211"/>
       <c r="F14" s="2" t="s">
         <v>62</v>
       </c>
@@ -8032,7 +8164,7 @@
       <c r="J14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="211"/>
+      <c r="K14" s="208"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -8042,7 +8174,7 @@
         <f>'Principal - ABP'!F19</f>
         <v>1</v>
       </c>
-      <c r="E15" s="208"/>
+      <c r="E15" s="211"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -8058,7 +8190,7 @@
       <c r="J15" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="211"/>
+      <c r="K15" s="208"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -8068,7 +8200,7 @@
         <f>C9*C15</f>
         <v>120</v>
       </c>
-      <c r="E16" s="208"/>
+      <c r="E16" s="211"/>
       <c r="F16" s="2" t="s">
         <v>64</v>
       </c>
@@ -8084,7 +8216,7 @@
       <c r="J16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="212"/>
+      <c r="K16" s="214"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -8094,7 +8226,7 @@
         <f>(IF(C15=1,H21,IF(C15=2,H37,IF(C15=3,H55,IF(C15=4,H76,IF(C15=5,H97,H118))))))</f>
         <v>101</v>
       </c>
-      <c r="E17" s="208"/>
+      <c r="E17" s="211"/>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
@@ -8110,7 +8242,7 @@
       <c r="J17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="213" t="s">
+      <c r="K17" s="207" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8122,7 +8254,7 @@
         <f>C17/C16-1</f>
         <v>-0.15833333333333333</v>
       </c>
-      <c r="E18" s="208"/>
+      <c r="E18" s="211"/>
       <c r="F18" s="2" t="s">
         <v>66</v>
       </c>
@@ -8138,7 +8270,7 @@
       <c r="J18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K18" s="211"/>
+      <c r="K18" s="208"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -8148,7 +8280,7 @@
         <f>C15*10</f>
         <v>10</v>
       </c>
-      <c r="E19" s="208"/>
+      <c r="E19" s="211"/>
       <c r="F19" s="2" t="s">
         <v>67</v>
       </c>
@@ -8164,7 +8296,7 @@
       <c r="J19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="211"/>
+      <c r="K19" s="208"/>
     </row>
     <row r="20" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
@@ -8174,7 +8306,7 @@
         <f>IF(C15=1,I21,IF(C15=2,I37,IF(C15=3,I55,IF(C15=4,I76,IF(C15=5,I97,I118)))))</f>
         <v>10.000000000000002</v>
       </c>
-      <c r="E20" s="209"/>
+      <c r="E20" s="212"/>
       <c r="F20" s="4" t="s">
         <v>68</v>
       </c>
@@ -8190,7 +8322,7 @@
       <c r="J20" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="214"/>
+      <c r="K20" s="209"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
@@ -8217,7 +8349,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="207" t="s">
+      <c r="E23" s="210" t="s">
         <v>141</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -8235,12 +8367,12 @@
       <c r="J23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="210" t="s">
+      <c r="K23" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="208"/>
+      <c r="E24" s="211"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
@@ -8256,10 +8388,10 @@
       <c r="J24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="211"/>
+      <c r="K24" s="208"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="208"/>
+      <c r="E25" s="211"/>
       <c r="F25" s="2" t="s">
         <v>58</v>
       </c>
@@ -8275,10 +8407,10 @@
       <c r="J25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K25" s="212"/>
+      <c r="K25" s="214"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="208"/>
+      <c r="E26" s="211"/>
       <c r="F26" s="2" t="s">
         <v>59</v>
       </c>
@@ -8294,12 +8426,12 @@
       <c r="J26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="213" t="s">
+      <c r="K26" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="208"/>
+      <c r="E27" s="211"/>
       <c r="F27" s="2" t="s">
         <v>60</v>
       </c>
@@ -8315,10 +8447,10 @@
       <c r="J27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="211"/>
+      <c r="K27" s="208"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="208"/>
+      <c r="E28" s="211"/>
       <c r="F28" s="2" t="s">
         <v>61</v>
       </c>
@@ -8334,10 +8466,10 @@
       <c r="J28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="211"/>
+      <c r="K28" s="208"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="208"/>
+      <c r="E29" s="211"/>
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
@@ -8353,10 +8485,10 @@
       <c r="J29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="211"/>
+      <c r="K29" s="208"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="208"/>
+      <c r="E30" s="211"/>
       <c r="F30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8372,10 +8504,10 @@
       <c r="J30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="211"/>
+      <c r="K30" s="208"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="208"/>
+      <c r="E31" s="211"/>
       <c r="F31" s="2" t="s">
         <v>64</v>
       </c>
@@ -8391,10 +8523,10 @@
       <c r="J31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K31" s="211"/>
+      <c r="K31" s="208"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="208"/>
+      <c r="E32" s="211"/>
       <c r="F32" s="2" t="s">
         <v>65</v>
       </c>
@@ -8410,10 +8542,10 @@
       <c r="J32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="212"/>
+      <c r="K32" s="214"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E33" s="208"/>
+      <c r="E33" s="211"/>
       <c r="F33" s="2" t="s">
         <v>66</v>
       </c>
@@ -8429,12 +8561,12 @@
       <c r="J33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K33" s="213" t="s">
+      <c r="K33" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" s="208"/>
+      <c r="E34" s="211"/>
       <c r="F34" s="2" t="s">
         <v>67</v>
       </c>
@@ -8450,10 +8582,10 @@
       <c r="J34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K34" s="211"/>
+      <c r="K34" s="208"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E35" s="208"/>
+      <c r="E35" s="211"/>
       <c r="F35" s="2" t="s">
         <v>68</v>
       </c>
@@ -8469,10 +8601,10 @@
       <c r="J35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K35" s="211"/>
+      <c r="K35" s="208"/>
     </row>
     <row r="36" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="209"/>
+      <c r="E36" s="212"/>
       <c r="F36" s="4" t="s">
         <v>69</v>
       </c>
@@ -8488,7 +8620,7 @@
       <c r="J36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K36" s="214"/>
+      <c r="K36" s="209"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
@@ -8515,7 +8647,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E39" s="207" t="s">
+      <c r="E39" s="210" t="s">
         <v>142</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -8533,12 +8665,12 @@
       <c r="J39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K39" s="210" t="s">
+      <c r="K39" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E40" s="208"/>
+      <c r="E40" s="211"/>
       <c r="F40" s="2" t="s">
         <v>57</v>
       </c>
@@ -8554,10 +8686,10 @@
       <c r="J40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K40" s="211"/>
+      <c r="K40" s="208"/>
     </row>
     <row r="41" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E41" s="208"/>
+      <c r="E41" s="211"/>
       <c r="F41" s="2" t="s">
         <v>58</v>
       </c>
@@ -8573,10 +8705,10 @@
       <c r="J41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K41" s="212"/>
+      <c r="K41" s="214"/>
     </row>
     <row r="42" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E42" s="208"/>
+      <c r="E42" s="211"/>
       <c r="F42" s="2" t="s">
         <v>59</v>
       </c>
@@ -8592,12 +8724,12 @@
       <c r="J42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K42" s="213" t="s">
+      <c r="K42" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E43" s="208"/>
+      <c r="E43" s="211"/>
       <c r="F43" s="2" t="s">
         <v>60</v>
       </c>
@@ -8613,10 +8745,10 @@
       <c r="J43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K43" s="211"/>
+      <c r="K43" s="208"/>
     </row>
     <row r="44" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E44" s="208"/>
+      <c r="E44" s="211"/>
       <c r="F44" s="2" t="s">
         <v>61</v>
       </c>
@@ -8632,10 +8764,10 @@
       <c r="J44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K44" s="211"/>
+      <c r="K44" s="208"/>
     </row>
     <row r="45" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E45" s="208"/>
+      <c r="E45" s="211"/>
       <c r="F45" s="2" t="s">
         <v>62</v>
       </c>
@@ -8651,10 +8783,10 @@
       <c r="J45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K45" s="211"/>
+      <c r="K45" s="208"/>
     </row>
     <row r="46" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E46" s="208"/>
+      <c r="E46" s="211"/>
       <c r="F46" s="2" t="s">
         <v>63</v>
       </c>
@@ -8670,10 +8802,10 @@
       <c r="J46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K46" s="211"/>
+      <c r="K46" s="208"/>
     </row>
     <row r="47" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E47" s="208"/>
+      <c r="E47" s="211"/>
       <c r="F47" s="2" t="s">
         <v>64</v>
       </c>
@@ -8689,10 +8821,10 @@
       <c r="J47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K47" s="211"/>
+      <c r="K47" s="208"/>
     </row>
     <row r="48" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E48" s="208"/>
+      <c r="E48" s="211"/>
       <c r="F48" s="2" t="s">
         <v>65</v>
       </c>
@@ -8708,10 +8840,10 @@
       <c r="J48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K48" s="211"/>
+      <c r="K48" s="208"/>
     </row>
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E49" s="208"/>
+      <c r="E49" s="211"/>
       <c r="F49" s="2" t="s">
         <v>66</v>
       </c>
@@ -8727,10 +8859,10 @@
       <c r="J49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K49" s="211"/>
+      <c r="K49" s="208"/>
     </row>
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E50" s="208"/>
+      <c r="E50" s="211"/>
       <c r="F50" s="2" t="s">
         <v>67</v>
       </c>
@@ -8746,10 +8878,10 @@
       <c r="J50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K50" s="212"/>
+      <c r="K50" s="214"/>
     </row>
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E51" s="208"/>
+      <c r="E51" s="211"/>
       <c r="F51" s="2" t="s">
         <v>68</v>
       </c>
@@ -8765,12 +8897,12 @@
       <c r="J51" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K51" s="213" t="s">
+      <c r="K51" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E52" s="208"/>
+      <c r="E52" s="211"/>
       <c r="F52" s="2" t="s">
         <v>69</v>
       </c>
@@ -8786,10 +8918,10 @@
       <c r="J52" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K52" s="211"/>
+      <c r="K52" s="208"/>
     </row>
     <row r="53" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E53" s="208"/>
+      <c r="E53" s="211"/>
       <c r="F53" s="2" t="s">
         <v>70</v>
       </c>
@@ -8805,10 +8937,10 @@
       <c r="J53" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K53" s="211"/>
+      <c r="K53" s="208"/>
     </row>
     <row r="54" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="209"/>
+      <c r="E54" s="212"/>
       <c r="F54" s="4" t="s">
         <v>71</v>
       </c>
@@ -8824,7 +8956,7 @@
       <c r="J54" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K54" s="214"/>
+      <c r="K54" s="209"/>
     </row>
     <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
@@ -8851,7 +8983,7 @@
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E57" s="207" t="s">
+      <c r="E57" s="210" t="s">
         <v>143</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -8869,12 +9001,12 @@
       <c r="J57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K57" s="210" t="s">
+      <c r="K57" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E58" s="208"/>
+      <c r="E58" s="211"/>
       <c r="F58" s="2" t="s">
         <v>57</v>
       </c>
@@ -8890,10 +9022,10 @@
       <c r="J58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K58" s="211"/>
+      <c r="K58" s="208"/>
     </row>
     <row r="59" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E59" s="208"/>
+      <c r="E59" s="211"/>
       <c r="F59" s="2" t="s">
         <v>58</v>
       </c>
@@ -8909,10 +9041,10 @@
       <c r="J59" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K59" s="212"/>
+      <c r="K59" s="214"/>
     </row>
     <row r="60" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E60" s="208"/>
+      <c r="E60" s="211"/>
       <c r="F60" s="2" t="s">
         <v>59</v>
       </c>
@@ -8928,12 +9060,12 @@
       <c r="J60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K60" s="213" t="s">
+      <c r="K60" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E61" s="208"/>
+      <c r="E61" s="211"/>
       <c r="F61" s="2" t="s">
         <v>60</v>
       </c>
@@ -8949,10 +9081,10 @@
       <c r="J61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K61" s="211"/>
+      <c r="K61" s="208"/>
     </row>
     <row r="62" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E62" s="208"/>
+      <c r="E62" s="211"/>
       <c r="F62" s="2" t="s">
         <v>61</v>
       </c>
@@ -8968,10 +9100,10 @@
       <c r="J62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K62" s="211"/>
+      <c r="K62" s="208"/>
     </row>
     <row r="63" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E63" s="208"/>
+      <c r="E63" s="211"/>
       <c r="F63" s="2" t="s">
         <v>62</v>
       </c>
@@ -8987,10 +9119,10 @@
       <c r="J63" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K63" s="211"/>
+      <c r="K63" s="208"/>
     </row>
     <row r="64" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="208"/>
+      <c r="E64" s="211"/>
       <c r="F64" s="2" t="s">
         <v>63</v>
       </c>
@@ -9006,10 +9138,10 @@
       <c r="J64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K64" s="211"/>
+      <c r="K64" s="208"/>
     </row>
     <row r="65" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E65" s="208"/>
+      <c r="E65" s="211"/>
       <c r="F65" s="2" t="s">
         <v>64</v>
       </c>
@@ -9025,10 +9157,10 @@
       <c r="J65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K65" s="211"/>
+      <c r="K65" s="208"/>
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E66" s="208"/>
+      <c r="E66" s="211"/>
       <c r="F66" s="2" t="s">
         <v>65</v>
       </c>
@@ -9044,10 +9176,10 @@
       <c r="J66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K66" s="211"/>
+      <c r="K66" s="208"/>
     </row>
     <row r="67" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E67" s="208"/>
+      <c r="E67" s="211"/>
       <c r="F67" s="2" t="s">
         <v>66</v>
       </c>
@@ -9063,10 +9195,10 @@
       <c r="J67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K67" s="211"/>
+      <c r="K67" s="208"/>
     </row>
     <row r="68" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E68" s="208"/>
+      <c r="E68" s="211"/>
       <c r="F68" s="2" t="s">
         <v>67</v>
       </c>
@@ -9082,10 +9214,10 @@
       <c r="J68" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K68" s="211"/>
+      <c r="K68" s="208"/>
     </row>
     <row r="69" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E69" s="208"/>
+      <c r="E69" s="211"/>
       <c r="F69" s="2" t="s">
         <v>68</v>
       </c>
@@ -9101,10 +9233,10 @@
       <c r="J69" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K69" s="211"/>
+      <c r="K69" s="208"/>
     </row>
     <row r="70" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E70" s="208"/>
+      <c r="E70" s="211"/>
       <c r="F70" s="2" t="s">
         <v>69</v>
       </c>
@@ -9120,10 +9252,10 @@
       <c r="J70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K70" s="211"/>
+      <c r="K70" s="208"/>
     </row>
     <row r="71" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E71" s="208"/>
+      <c r="E71" s="211"/>
       <c r="F71" s="2" t="s">
         <v>70</v>
       </c>
@@ -9139,10 +9271,10 @@
       <c r="J71" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K71" s="212"/>
+      <c r="K71" s="214"/>
     </row>
     <row r="72" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E72" s="208"/>
+      <c r="E72" s="211"/>
       <c r="F72" s="2" t="s">
         <v>71</v>
       </c>
@@ -9158,12 +9290,12 @@
       <c r="J72" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K72" s="213" t="s">
+      <c r="K72" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E73" s="208"/>
+      <c r="E73" s="211"/>
       <c r="F73" s="2" t="s">
         <v>72</v>
       </c>
@@ -9179,10 +9311,10 @@
       <c r="J73" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K73" s="211"/>
+      <c r="K73" s="208"/>
     </row>
     <row r="74" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E74" s="208"/>
+      <c r="E74" s="211"/>
       <c r="F74" s="2" t="s">
         <v>73</v>
       </c>
@@ -9198,10 +9330,10 @@
       <c r="J74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K74" s="211"/>
+      <c r="K74" s="208"/>
     </row>
     <row r="75" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E75" s="209"/>
+      <c r="E75" s="212"/>
       <c r="F75" s="4" t="s">
         <v>74</v>
       </c>
@@ -9217,7 +9349,7 @@
       <c r="J75" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K75" s="214"/>
+      <c r="K75" s="209"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
@@ -9237,7 +9369,7 @@
     </row>
     <row r="77" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E78" s="207" t="s">
+      <c r="E78" s="210" t="s">
         <v>144</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -9260,7 +9392,7 @@
       </c>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E79" s="208"/>
+      <c r="E79" s="211"/>
       <c r="F79" s="2" t="s">
         <v>57</v>
       </c>
@@ -9279,7 +9411,7 @@
       <c r="K79" s="216"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E80" s="208"/>
+      <c r="E80" s="211"/>
       <c r="F80" s="2" t="s">
         <v>58</v>
       </c>
@@ -9298,7 +9430,7 @@
       <c r="K80" s="217"/>
     </row>
     <row r="81" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E81" s="208"/>
+      <c r="E81" s="211"/>
       <c r="F81" s="2" t="s">
         <v>59</v>
       </c>
@@ -9314,12 +9446,12 @@
       <c r="J81" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K81" s="213" t="s">
+      <c r="K81" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E82" s="208"/>
+      <c r="E82" s="211"/>
       <c r="F82" s="2" t="s">
         <v>60</v>
       </c>
@@ -9335,10 +9467,10 @@
       <c r="J82" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K82" s="211"/>
+      <c r="K82" s="208"/>
     </row>
     <row r="83" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E83" s="208"/>
+      <c r="E83" s="211"/>
       <c r="F83" s="2" t="s">
         <v>61</v>
       </c>
@@ -9354,10 +9486,10 @@
       <c r="J83" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K83" s="211"/>
+      <c r="K83" s="208"/>
     </row>
     <row r="84" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E84" s="208"/>
+      <c r="E84" s="211"/>
       <c r="F84" s="2" t="s">
         <v>62</v>
       </c>
@@ -9373,10 +9505,10 @@
       <c r="J84" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K84" s="211"/>
+      <c r="K84" s="208"/>
     </row>
     <row r="85" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E85" s="208"/>
+      <c r="E85" s="211"/>
       <c r="F85" s="2" t="s">
         <v>63</v>
       </c>
@@ -9392,10 +9524,10 @@
       <c r="J85" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K85" s="211"/>
+      <c r="K85" s="208"/>
     </row>
     <row r="86" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E86" s="208"/>
+      <c r="E86" s="211"/>
       <c r="F86" s="2" t="s">
         <v>64</v>
       </c>
@@ -9411,10 +9543,10 @@
       <c r="J86" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K86" s="211"/>
+      <c r="K86" s="208"/>
     </row>
     <row r="87" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E87" s="208"/>
+      <c r="E87" s="211"/>
       <c r="F87" s="2" t="s">
         <v>65</v>
       </c>
@@ -9430,10 +9562,10 @@
       <c r="J87" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K87" s="211"/>
+      <c r="K87" s="208"/>
     </row>
     <row r="88" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E88" s="208"/>
+      <c r="E88" s="211"/>
       <c r="F88" s="2" t="s">
         <v>66</v>
       </c>
@@ -9449,10 +9581,10 @@
       <c r="J88" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K88" s="211"/>
+      <c r="K88" s="208"/>
     </row>
     <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="208"/>
+      <c r="E89" s="211"/>
       <c r="F89" s="2" t="s">
         <v>67</v>
       </c>
@@ -9468,10 +9600,10 @@
       <c r="J89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K89" s="211"/>
+      <c r="K89" s="208"/>
     </row>
     <row r="90" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E90" s="208"/>
+      <c r="E90" s="211"/>
       <c r="F90" s="2" t="s">
         <v>68</v>
       </c>
@@ -9487,10 +9619,10 @@
       <c r="J90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K90" s="211"/>
+      <c r="K90" s="208"/>
     </row>
     <row r="91" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E91" s="208"/>
+      <c r="E91" s="211"/>
       <c r="F91" s="2" t="s">
         <v>69</v>
       </c>
@@ -9506,10 +9638,10 @@
       <c r="J91" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K91" s="211"/>
+      <c r="K91" s="208"/>
     </row>
     <row r="92" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E92" s="208"/>
+      <c r="E92" s="211"/>
       <c r="F92" s="2" t="s">
         <v>70</v>
       </c>
@@ -9525,10 +9657,10 @@
       <c r="J92" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K92" s="211"/>
+      <c r="K92" s="208"/>
     </row>
     <row r="93" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E93" s="208"/>
+      <c r="E93" s="211"/>
       <c r="F93" s="2" t="s">
         <v>71</v>
       </c>
@@ -9544,10 +9676,10 @@
       <c r="J93" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K93" s="212"/>
+      <c r="K93" s="214"/>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E94" s="208"/>
+      <c r="E94" s="211"/>
       <c r="F94" s="2" t="s">
         <v>72</v>
       </c>
@@ -9563,12 +9695,12 @@
       <c r="J94" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K94" s="213" t="s">
+      <c r="K94" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E95" s="208"/>
+      <c r="E95" s="211"/>
       <c r="F95" s="2" t="s">
         <v>73</v>
       </c>
@@ -9584,10 +9716,10 @@
       <c r="J95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K95" s="211"/>
+      <c r="K95" s="208"/>
     </row>
     <row r="96" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E96" s="209"/>
+      <c r="E96" s="212"/>
       <c r="F96" s="4" t="s">
         <v>74</v>
       </c>
@@ -9603,7 +9735,7 @@
       <c r="J96" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K96" s="214"/>
+      <c r="K96" s="209"/>
     </row>
     <row r="97" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
@@ -9623,7 +9755,7 @@
     </row>
     <row r="98" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E99" s="207" t="s">
+      <c r="E99" s="210" t="s">
         <v>145</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -9641,12 +9773,12 @@
       <c r="J99" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K99" s="210" t="s">
+      <c r="K99" s="213" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="100" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E100" s="208"/>
+      <c r="E100" s="211"/>
       <c r="F100" s="2" t="s">
         <v>57</v>
       </c>
@@ -9662,10 +9794,10 @@
       <c r="J100" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K100" s="211"/>
+      <c r="K100" s="208"/>
     </row>
     <row r="101" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E101" s="208"/>
+      <c r="E101" s="211"/>
       <c r="F101" s="2" t="s">
         <v>58</v>
       </c>
@@ -9681,10 +9813,10 @@
       <c r="J101" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K101" s="212"/>
+      <c r="K101" s="214"/>
     </row>
     <row r="102" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E102" s="208"/>
+      <c r="E102" s="211"/>
       <c r="F102" s="2" t="s">
         <v>59</v>
       </c>
@@ -9700,12 +9832,12 @@
       <c r="J102" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K102" s="213" t="s">
+      <c r="K102" s="207" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="103" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E103" s="208"/>
+      <c r="E103" s="211"/>
       <c r="F103" s="2" t="s">
         <v>60</v>
       </c>
@@ -9721,10 +9853,10 @@
       <c r="J103" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K103" s="211"/>
+      <c r="K103" s="208"/>
     </row>
     <row r="104" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E104" s="208"/>
+      <c r="E104" s="211"/>
       <c r="F104" s="2" t="s">
         <v>61</v>
       </c>
@@ -9740,10 +9872,10 @@
       <c r="J104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K104" s="211"/>
+      <c r="K104" s="208"/>
     </row>
     <row r="105" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E105" s="208"/>
+      <c r="E105" s="211"/>
       <c r="F105" s="2" t="s">
         <v>62</v>
       </c>
@@ -9759,10 +9891,10 @@
       <c r="J105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K105" s="211"/>
+      <c r="K105" s="208"/>
     </row>
     <row r="106" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E106" s="208"/>
+      <c r="E106" s="211"/>
       <c r="F106" s="2" t="s">
         <v>63</v>
       </c>
@@ -9778,10 +9910,10 @@
       <c r="J106" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K106" s="211"/>
+      <c r="K106" s="208"/>
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E107" s="208"/>
+      <c r="E107" s="211"/>
       <c r="F107" s="2" t="s">
         <v>64</v>
       </c>
@@ -9797,10 +9929,10 @@
       <c r="J107" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K107" s="211"/>
+      <c r="K107" s="208"/>
     </row>
     <row r="108" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E108" s="208"/>
+      <c r="E108" s="211"/>
       <c r="F108" s="2" t="s">
         <v>65</v>
       </c>
@@ -9816,10 +9948,10 @@
       <c r="J108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K108" s="211"/>
+      <c r="K108" s="208"/>
     </row>
     <row r="109" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E109" s="208"/>
+      <c r="E109" s="211"/>
       <c r="F109" s="2" t="s">
         <v>66</v>
       </c>
@@ -9835,10 +9967,10 @@
       <c r="J109" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K109" s="211"/>
+      <c r="K109" s="208"/>
     </row>
     <row r="110" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E110" s="208"/>
+      <c r="E110" s="211"/>
       <c r="F110" s="2" t="s">
         <v>67</v>
       </c>
@@ -9854,10 +9986,10 @@
       <c r="J110" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K110" s="211"/>
+      <c r="K110" s="208"/>
     </row>
     <row r="111" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E111" s="208"/>
+      <c r="E111" s="211"/>
       <c r="F111" s="2" t="s">
         <v>68</v>
       </c>
@@ -9873,10 +10005,10 @@
       <c r="J111" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K111" s="211"/>
+      <c r="K111" s="208"/>
     </row>
     <row r="112" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E112" s="208"/>
+      <c r="E112" s="211"/>
       <c r="F112" s="2" t="s">
         <v>69</v>
       </c>
@@ -9892,10 +10024,10 @@
       <c r="J112" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K112" s="211"/>
+      <c r="K112" s="208"/>
     </row>
     <row r="113" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E113" s="208"/>
+      <c r="E113" s="211"/>
       <c r="F113" s="2" t="s">
         <v>70</v>
       </c>
@@ -9911,10 +10043,10 @@
       <c r="J113" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K113" s="211"/>
+      <c r="K113" s="208"/>
     </row>
     <row r="114" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E114" s="208"/>
+      <c r="E114" s="211"/>
       <c r="F114" s="2" t="s">
         <v>71</v>
       </c>
@@ -9930,10 +10062,10 @@
       <c r="J114" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K114" s="211"/>
+      <c r="K114" s="208"/>
     </row>
     <row r="115" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E115" s="208"/>
+      <c r="E115" s="211"/>
       <c r="F115" s="2" t="s">
         <v>72</v>
       </c>
@@ -9949,10 +10081,10 @@
       <c r="J115" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K115" s="212"/>
+      <c r="K115" s="214"/>
     </row>
     <row r="116" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E116" s="208"/>
+      <c r="E116" s="211"/>
       <c r="F116" s="2" t="s">
         <v>73</v>
       </c>
@@ -9968,12 +10100,12 @@
       <c r="J116" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K116" s="213" t="s">
+      <c r="K116" s="207" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="209"/>
+      <c r="E117" s="212"/>
       <c r="F117" s="4" t="s">
         <v>74</v>
       </c>
@@ -9989,7 +10121,7 @@
       <c r="J117" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K117" s="214"/>
+      <c r="K117" s="209"/>
     </row>
     <row r="118" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F118" s="1"/>
@@ -10010,18 +10142,6 @@
   </sheetData>
   <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="E8:E20"/>
-    <mergeCell ref="E23:E36"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K16"/>
-    <mergeCell ref="K17:K20"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="K26:K32"/>
     <mergeCell ref="E99:E117"/>
     <mergeCell ref="K99:K101"/>
     <mergeCell ref="K102:K115"/>
@@ -10038,6 +10158,18 @@
     <mergeCell ref="E39:E54"/>
     <mergeCell ref="E57:E75"/>
     <mergeCell ref="E78:E96"/>
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="E8:E20"/>
+    <mergeCell ref="E23:E36"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K26:K32"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:K21">
     <cfRule type="expression" dxfId="63" priority="7">
@@ -13605,6 +13737,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14209,7 +14353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O58"/>
   <sheetViews>
@@ -15203,123 +15347,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="190" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="192"/>
-    </row>
-    <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="232" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="233"/>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
-      <c r="I3" s="233"/>
-      <c r="J3" s="233"/>
-      <c r="K3" s="234"/>
-    </row>
-    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="6">
-        <f>SUM(C6:C8)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="25" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="6">
-        <f>'Principal - ABP'!L19</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="6">
-        <f>C13*10</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Añadida entrega final de la asignatura PostProducción Digital
</commit_message>
<xml_diff>
--- a/documentos/plantilla ABP.xlsx
+++ b/documentos/plantilla ABP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="500" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="500" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Principal - ABP" sheetId="1" r:id="rId1"/>
@@ -18,24 +18,23 @@
     <sheet name="V1" sheetId="6" r:id="rId4"/>
     <sheet name="V2" sheetId="7" r:id="rId5"/>
     <sheet name="PD" sheetId="2" r:id="rId6"/>
-    <sheet name="Hoja1" sheetId="18" r:id="rId7"/>
-    <sheet name="TDS" sheetId="10" r:id="rId8"/>
-    <sheet name="RV" sheetId="11" r:id="rId9"/>
-    <sheet name="SMBI" sheetId="8" r:id="rId10"/>
-    <sheet name="EL" sheetId="12" r:id="rId11"/>
-    <sheet name="SDM" sheetId="13" r:id="rId12"/>
-    <sheet name="SMA" sheetId="14" r:id="rId13"/>
-    <sheet name="PD1" sheetId="17" r:id="rId14"/>
-    <sheet name="NM" sheetId="15" r:id="rId15"/>
-    <sheet name="Hoja2" sheetId="19" r:id="rId16"/>
+    <sheet name="TDS" sheetId="10" r:id="rId7"/>
+    <sheet name="RV" sheetId="11" r:id="rId8"/>
+    <sheet name="SMBI" sheetId="8" r:id="rId9"/>
+    <sheet name="EL" sheetId="12" r:id="rId10"/>
+    <sheet name="SDM" sheetId="13" r:id="rId11"/>
+    <sheet name="SMA" sheetId="14" r:id="rId12"/>
+    <sheet name="PD1" sheetId="17" r:id="rId13"/>
+    <sheet name="NM" sheetId="15" r:id="rId14"/>
+    <sheet name="Hoja2" sheetId="19" r:id="rId15"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
     <definedName name="Graficos1">TAG!$F$8:$H$21</definedName>
   </definedNames>
-  <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3437,15 +3436,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3458,7 +3448,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5233,13 +5232,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="190" t="s">
-        <v>234</v>
+        <v>364</v>
       </c>
       <c r="C2" s="191"/>
       <c r="D2" s="191"/>
@@ -5267,7 +5266,7 @@
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>236</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -5305,7 +5304,7 @@
     </row>
     <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>239</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -5313,8 +5312,8 @@
         <v>110</v>
       </c>
       <c r="C13" s="6">
-        <f>'Principal - ABP'!L19</f>
-        <v>1</v>
+        <f>'Principal - ABP'!M19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -5323,7 +5322,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5333,7 +5332,6 @@
     <mergeCell ref="B3:K3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5358,7 +5356,7 @@
     <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="190" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C2" s="191"/>
       <c r="D2" s="191"/>
@@ -5386,7 +5384,7 @@
     </row>
     <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
@@ -5424,7 +5422,7 @@
     </row>
     <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
@@ -5432,8 +5430,8 @@
         <v>110</v>
       </c>
       <c r="C13" s="6">
-        <f>'Principal - ABP'!M19</f>
-        <v>0</v>
+        <f>'Principal - ABP'!N19</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
@@ -5442,7 +5440,7 @@
       </c>
       <c r="C14" s="6">
         <f>C13*10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5461,124 +5459,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="190" t="s">
-        <v>367</v>
-      </c>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="192"/>
-    </row>
-    <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="232" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="233"/>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
-      <c r="I3" s="233"/>
-      <c r="J3" s="233"/>
-      <c r="K3" s="234"/>
-    </row>
-    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C7" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="6">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="6">
-        <f>SUM(C6:C8)</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="25" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="6">
-        <f>'Principal - ABP'!N19</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="6">
-        <f>C13*10</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P21"/>
   <sheetViews>
@@ -6062,12 +5942,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6138,7 +6018,7 @@
       <c r="I4" s="163"/>
       <c r="J4" s="163"/>
       <c r="K4" s="167">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6180,7 +6060,7 @@
       <c r="I6" s="165"/>
       <c r="J6" s="165"/>
       <c r="K6" s="166">
-        <v>0.55000000000000004</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -6194,7 +6074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K14"/>
   <sheetViews>
@@ -6312,7 +6192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -7911,7 +7791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" workbookViewId="0">
+    <sheetView topLeftCell="F63" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -8006,7 +7886,7 @@
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="E8" s="210" t="s">
+      <c r="E8" s="207" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -8024,7 +7904,7 @@
       <c r="J8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="213" t="s">
+      <c r="K8" s="210" t="s">
         <v>8</v>
       </c>
     </row>
@@ -8035,7 +7915,7 @@
       <c r="C9" s="6">
         <v>120</v>
       </c>
-      <c r="E9" s="211"/>
+      <c r="E9" s="208"/>
       <c r="F9" s="2" t="s">
         <v>57</v>
       </c>
@@ -8051,7 +7931,7 @@
       <c r="J9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="208"/>
+      <c r="K9" s="211"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
@@ -8060,7 +7940,7 @@
       <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="211"/>
+      <c r="E10" s="208"/>
       <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
@@ -8076,7 +7956,7 @@
       <c r="J10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="214"/>
+      <c r="K10" s="212"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
@@ -8086,7 +7966,7 @@
         <f>SUM(C8:C10)</f>
         <v>150</v>
       </c>
-      <c r="E11" s="211"/>
+      <c r="E11" s="208"/>
       <c r="F11" s="2" t="s">
         <v>59</v>
       </c>
@@ -8102,12 +7982,12 @@
       <c r="J11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="207" t="s">
+      <c r="K11" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="211"/>
+      <c r="E12" s="208"/>
       <c r="F12" s="2" t="s">
         <v>60</v>
       </c>
@@ -8123,10 +8003,10 @@
       <c r="J12" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="208"/>
+      <c r="K12" s="211"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="211"/>
+      <c r="E13" s="208"/>
       <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
@@ -8142,13 +8022,13 @@
       <c r="J13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K13" s="208"/>
+      <c r="K13" s="211"/>
     </row>
     <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="211"/>
+      <c r="E14" s="208"/>
       <c r="F14" s="2" t="s">
         <v>62</v>
       </c>
@@ -8164,7 +8044,7 @@
       <c r="J14" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="208"/>
+      <c r="K14" s="211"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -8174,7 +8054,7 @@
         <f>'Principal - ABP'!F19</f>
         <v>1</v>
       </c>
-      <c r="E15" s="211"/>
+      <c r="E15" s="208"/>
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
@@ -8190,7 +8070,7 @@
       <c r="J15" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="208"/>
+      <c r="K15" s="211"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -8200,7 +8080,7 @@
         <f>C9*C15</f>
         <v>120</v>
       </c>
-      <c r="E16" s="211"/>
+      <c r="E16" s="208"/>
       <c r="F16" s="2" t="s">
         <v>64</v>
       </c>
@@ -8216,7 +8096,7 @@
       <c r="J16" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="214"/>
+      <c r="K16" s="212"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -8226,7 +8106,7 @@
         <f>(IF(C15=1,H21,IF(C15=2,H37,IF(C15=3,H55,IF(C15=4,H76,IF(C15=5,H97,H118))))))</f>
         <v>101</v>
       </c>
-      <c r="E17" s="211"/>
+      <c r="E17" s="208"/>
       <c r="F17" s="2" t="s">
         <v>65</v>
       </c>
@@ -8242,7 +8122,7 @@
       <c r="J17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="207" t="s">
+      <c r="K17" s="213" t="s">
         <v>10</v>
       </c>
     </row>
@@ -8254,7 +8134,7 @@
         <f>C17/C16-1</f>
         <v>-0.15833333333333333</v>
       </c>
-      <c r="E18" s="211"/>
+      <c r="E18" s="208"/>
       <c r="F18" s="2" t="s">
         <v>66</v>
       </c>
@@ -8270,7 +8150,7 @@
       <c r="J18" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K18" s="208"/>
+      <c r="K18" s="211"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -8280,7 +8160,7 @@
         <f>C15*10</f>
         <v>10</v>
       </c>
-      <c r="E19" s="211"/>
+      <c r="E19" s="208"/>
       <c r="F19" s="2" t="s">
         <v>67</v>
       </c>
@@ -8296,7 +8176,7 @@
       <c r="J19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K19" s="208"/>
+      <c r="K19" s="211"/>
     </row>
     <row r="20" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
@@ -8306,7 +8186,7 @@
         <f>IF(C15=1,I21,IF(C15=2,I37,IF(C15=3,I55,IF(C15=4,I76,IF(C15=5,I97,I118)))))</f>
         <v>10.000000000000002</v>
       </c>
-      <c r="E20" s="212"/>
+      <c r="E20" s="209"/>
       <c r="F20" s="4" t="s">
         <v>68</v>
       </c>
@@ -8322,7 +8202,7 @@
       <c r="J20" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K20" s="209"/>
+      <c r="K20" s="214"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
@@ -8349,7 +8229,7 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="210" t="s">
+      <c r="E23" s="207" t="s">
         <v>141</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -8367,12 +8247,12 @@
       <c r="J23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="213" t="s">
+      <c r="K23" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="211"/>
+      <c r="E24" s="208"/>
       <c r="F24" s="2" t="s">
         <v>57</v>
       </c>
@@ -8388,10 +8268,10 @@
       <c r="J24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="208"/>
+      <c r="K24" s="211"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="211"/>
+      <c r="E25" s="208"/>
       <c r="F25" s="2" t="s">
         <v>58</v>
       </c>
@@ -8407,10 +8287,10 @@
       <c r="J25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K25" s="214"/>
+      <c r="K25" s="212"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="211"/>
+      <c r="E26" s="208"/>
       <c r="F26" s="2" t="s">
         <v>59</v>
       </c>
@@ -8426,12 +8306,12 @@
       <c r="J26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K26" s="207" t="s">
+      <c r="K26" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="211"/>
+      <c r="E27" s="208"/>
       <c r="F27" s="2" t="s">
         <v>60</v>
       </c>
@@ -8447,10 +8327,10 @@
       <c r="J27" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="208"/>
+      <c r="K27" s="211"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="211"/>
+      <c r="E28" s="208"/>
       <c r="F28" s="2" t="s">
         <v>61</v>
       </c>
@@ -8466,10 +8346,10 @@
       <c r="J28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="208"/>
+      <c r="K28" s="211"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="211"/>
+      <c r="E29" s="208"/>
       <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
@@ -8485,10 +8365,10 @@
       <c r="J29" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="208"/>
+      <c r="K29" s="211"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="211"/>
+      <c r="E30" s="208"/>
       <c r="F30" s="2" t="s">
         <v>63</v>
       </c>
@@ -8504,10 +8384,10 @@
       <c r="J30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="208"/>
+      <c r="K30" s="211"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="211"/>
+      <c r="E31" s="208"/>
       <c r="F31" s="2" t="s">
         <v>64</v>
       </c>
@@ -8523,10 +8403,10 @@
       <c r="J31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K31" s="208"/>
+      <c r="K31" s="211"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="211"/>
+      <c r="E32" s="208"/>
       <c r="F32" s="2" t="s">
         <v>65</v>
       </c>
@@ -8542,10 +8422,10 @@
       <c r="J32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="214"/>
+      <c r="K32" s="212"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E33" s="211"/>
+      <c r="E33" s="208"/>
       <c r="F33" s="2" t="s">
         <v>66</v>
       </c>
@@ -8561,12 +8441,12 @@
       <c r="J33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K33" s="207" t="s">
+      <c r="K33" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" s="211"/>
+      <c r="E34" s="208"/>
       <c r="F34" s="2" t="s">
         <v>67</v>
       </c>
@@ -8582,10 +8462,10 @@
       <c r="J34" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K34" s="208"/>
+      <c r="K34" s="211"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E35" s="211"/>
+      <c r="E35" s="208"/>
       <c r="F35" s="2" t="s">
         <v>68</v>
       </c>
@@ -8601,10 +8481,10 @@
       <c r="J35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K35" s="208"/>
+      <c r="K35" s="211"/>
     </row>
     <row r="36" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="212"/>
+      <c r="E36" s="209"/>
       <c r="F36" s="4" t="s">
         <v>69</v>
       </c>
@@ -8620,7 +8500,7 @@
       <c r="J36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K36" s="209"/>
+      <c r="K36" s="214"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
@@ -8647,7 +8527,7 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E39" s="210" t="s">
+      <c r="E39" s="207" t="s">
         <v>142</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -8665,12 +8545,12 @@
       <c r="J39" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K39" s="213" t="s">
+      <c r="K39" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E40" s="211"/>
+      <c r="E40" s="208"/>
       <c r="F40" s="2" t="s">
         <v>57</v>
       </c>
@@ -8686,10 +8566,10 @@
       <c r="J40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K40" s="208"/>
+      <c r="K40" s="211"/>
     </row>
     <row r="41" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E41" s="211"/>
+      <c r="E41" s="208"/>
       <c r="F41" s="2" t="s">
         <v>58</v>
       </c>
@@ -8705,10 +8585,10 @@
       <c r="J41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K41" s="214"/>
+      <c r="K41" s="212"/>
     </row>
     <row r="42" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E42" s="211"/>
+      <c r="E42" s="208"/>
       <c r="F42" s="2" t="s">
         <v>59</v>
       </c>
@@ -8724,12 +8604,12 @@
       <c r="J42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K42" s="207" t="s">
+      <c r="K42" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E43" s="211"/>
+      <c r="E43" s="208"/>
       <c r="F43" s="2" t="s">
         <v>60</v>
       </c>
@@ -8745,10 +8625,10 @@
       <c r="J43" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K43" s="208"/>
+      <c r="K43" s="211"/>
     </row>
     <row r="44" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E44" s="211"/>
+      <c r="E44" s="208"/>
       <c r="F44" s="2" t="s">
         <v>61</v>
       </c>
@@ -8764,10 +8644,10 @@
       <c r="J44" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K44" s="208"/>
+      <c r="K44" s="211"/>
     </row>
     <row r="45" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E45" s="211"/>
+      <c r="E45" s="208"/>
       <c r="F45" s="2" t="s">
         <v>62</v>
       </c>
@@ -8783,10 +8663,10 @@
       <c r="J45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K45" s="208"/>
+      <c r="K45" s="211"/>
     </row>
     <row r="46" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E46" s="211"/>
+      <c r="E46" s="208"/>
       <c r="F46" s="2" t="s">
         <v>63</v>
       </c>
@@ -8802,10 +8682,10 @@
       <c r="J46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K46" s="208"/>
+      <c r="K46" s="211"/>
     </row>
     <row r="47" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E47" s="211"/>
+      <c r="E47" s="208"/>
       <c r="F47" s="2" t="s">
         <v>64</v>
       </c>
@@ -8821,10 +8701,10 @@
       <c r="J47" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K47" s="208"/>
+      <c r="K47" s="211"/>
     </row>
     <row r="48" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E48" s="211"/>
+      <c r="E48" s="208"/>
       <c r="F48" s="2" t="s">
         <v>65</v>
       </c>
@@ -8840,10 +8720,10 @@
       <c r="J48" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K48" s="208"/>
+      <c r="K48" s="211"/>
     </row>
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E49" s="211"/>
+      <c r="E49" s="208"/>
       <c r="F49" s="2" t="s">
         <v>66</v>
       </c>
@@ -8859,10 +8739,10 @@
       <c r="J49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K49" s="208"/>
+      <c r="K49" s="211"/>
     </row>
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E50" s="211"/>
+      <c r="E50" s="208"/>
       <c r="F50" s="2" t="s">
         <v>67</v>
       </c>
@@ -8878,10 +8758,10 @@
       <c r="J50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K50" s="214"/>
+      <c r="K50" s="212"/>
     </row>
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E51" s="211"/>
+      <c r="E51" s="208"/>
       <c r="F51" s="2" t="s">
         <v>68</v>
       </c>
@@ -8897,12 +8777,12 @@
       <c r="J51" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K51" s="207" t="s">
+      <c r="K51" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E52" s="211"/>
+      <c r="E52" s="208"/>
       <c r="F52" s="2" t="s">
         <v>69</v>
       </c>
@@ -8918,10 +8798,10 @@
       <c r="J52" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K52" s="208"/>
+      <c r="K52" s="211"/>
     </row>
     <row r="53" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E53" s="211"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="2" t="s">
         <v>70</v>
       </c>
@@ -8937,10 +8817,10 @@
       <c r="J53" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K53" s="208"/>
+      <c r="K53" s="211"/>
     </row>
     <row r="54" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E54" s="212"/>
+      <c r="E54" s="209"/>
       <c r="F54" s="4" t="s">
         <v>71</v>
       </c>
@@ -8956,7 +8836,7 @@
       <c r="J54" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K54" s="209"/>
+      <c r="K54" s="214"/>
     </row>
     <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
@@ -8983,7 +8863,7 @@
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E57" s="210" t="s">
+      <c r="E57" s="207" t="s">
         <v>143</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -9001,12 +8881,12 @@
       <c r="J57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K57" s="213" t="s">
+      <c r="K57" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="58" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E58" s="211"/>
+      <c r="E58" s="208"/>
       <c r="F58" s="2" t="s">
         <v>57</v>
       </c>
@@ -9022,10 +8902,10 @@
       <c r="J58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K58" s="208"/>
+      <c r="K58" s="211"/>
     </row>
     <row r="59" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E59" s="211"/>
+      <c r="E59" s="208"/>
       <c r="F59" s="2" t="s">
         <v>58</v>
       </c>
@@ -9041,10 +8921,10 @@
       <c r="J59" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K59" s="214"/>
+      <c r="K59" s="212"/>
     </row>
     <row r="60" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E60" s="211"/>
+      <c r="E60" s="208"/>
       <c r="F60" s="2" t="s">
         <v>59</v>
       </c>
@@ -9060,12 +8940,12 @@
       <c r="J60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K60" s="207" t="s">
+      <c r="K60" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E61" s="211"/>
+      <c r="E61" s="208"/>
       <c r="F61" s="2" t="s">
         <v>60</v>
       </c>
@@ -9081,10 +8961,10 @@
       <c r="J61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K61" s="208"/>
+      <c r="K61" s="211"/>
     </row>
     <row r="62" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E62" s="211"/>
+      <c r="E62" s="208"/>
       <c r="F62" s="2" t="s">
         <v>61</v>
       </c>
@@ -9100,10 +8980,10 @@
       <c r="J62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K62" s="208"/>
+      <c r="K62" s="211"/>
     </row>
     <row r="63" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E63" s="211"/>
+      <c r="E63" s="208"/>
       <c r="F63" s="2" t="s">
         <v>62</v>
       </c>
@@ -9119,10 +8999,10 @@
       <c r="J63" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K63" s="208"/>
+      <c r="K63" s="211"/>
     </row>
     <row r="64" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="211"/>
+      <c r="E64" s="208"/>
       <c r="F64" s="2" t="s">
         <v>63</v>
       </c>
@@ -9138,10 +9018,10 @@
       <c r="J64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K64" s="208"/>
+      <c r="K64" s="211"/>
     </row>
     <row r="65" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E65" s="211"/>
+      <c r="E65" s="208"/>
       <c r="F65" s="2" t="s">
         <v>64</v>
       </c>
@@ -9157,10 +9037,10 @@
       <c r="J65" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K65" s="208"/>
+      <c r="K65" s="211"/>
     </row>
     <row r="66" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E66" s="211"/>
+      <c r="E66" s="208"/>
       <c r="F66" s="2" t="s">
         <v>65</v>
       </c>
@@ -9176,10 +9056,10 @@
       <c r="J66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K66" s="208"/>
+      <c r="K66" s="211"/>
     </row>
     <row r="67" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E67" s="211"/>
+      <c r="E67" s="208"/>
       <c r="F67" s="2" t="s">
         <v>66</v>
       </c>
@@ -9195,10 +9075,10 @@
       <c r="J67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K67" s="208"/>
+      <c r="K67" s="211"/>
     </row>
     <row r="68" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E68" s="211"/>
+      <c r="E68" s="208"/>
       <c r="F68" s="2" t="s">
         <v>67</v>
       </c>
@@ -9214,10 +9094,10 @@
       <c r="J68" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K68" s="208"/>
+      <c r="K68" s="211"/>
     </row>
     <row r="69" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E69" s="211"/>
+      <c r="E69" s="208"/>
       <c r="F69" s="2" t="s">
         <v>68</v>
       </c>
@@ -9233,10 +9113,10 @@
       <c r="J69" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K69" s="208"/>
+      <c r="K69" s="211"/>
     </row>
     <row r="70" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E70" s="211"/>
+      <c r="E70" s="208"/>
       <c r="F70" s="2" t="s">
         <v>69</v>
       </c>
@@ -9252,10 +9132,10 @@
       <c r="J70" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K70" s="208"/>
+      <c r="K70" s="211"/>
     </row>
     <row r="71" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E71" s="211"/>
+      <c r="E71" s="208"/>
       <c r="F71" s="2" t="s">
         <v>70</v>
       </c>
@@ -9271,10 +9151,10 @@
       <c r="J71" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K71" s="214"/>
+      <c r="K71" s="212"/>
     </row>
     <row r="72" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E72" s="211"/>
+      <c r="E72" s="208"/>
       <c r="F72" s="2" t="s">
         <v>71</v>
       </c>
@@ -9290,12 +9170,12 @@
       <c r="J72" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K72" s="207" t="s">
+      <c r="K72" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E73" s="211"/>
+      <c r="E73" s="208"/>
       <c r="F73" s="2" t="s">
         <v>72</v>
       </c>
@@ -9311,10 +9191,10 @@
       <c r="J73" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K73" s="208"/>
+      <c r="K73" s="211"/>
     </row>
     <row r="74" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E74" s="211"/>
+      <c r="E74" s="208"/>
       <c r="F74" s="2" t="s">
         <v>73</v>
       </c>
@@ -9330,10 +9210,10 @@
       <c r="J74" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K74" s="208"/>
+      <c r="K74" s="211"/>
     </row>
     <row r="75" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E75" s="212"/>
+      <c r="E75" s="209"/>
       <c r="F75" s="4" t="s">
         <v>74</v>
       </c>
@@ -9349,7 +9229,7 @@
       <c r="J75" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K75" s="209"/>
+      <c r="K75" s="214"/>
     </row>
     <row r="76" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
@@ -9369,7 +9249,7 @@
     </row>
     <row r="77" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E78" s="210" t="s">
+      <c r="E78" s="207" t="s">
         <v>144</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -9392,7 +9272,7 @@
       </c>
     </row>
     <row r="79" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E79" s="211"/>
+      <c r="E79" s="208"/>
       <c r="F79" s="2" t="s">
         <v>57</v>
       </c>
@@ -9411,7 +9291,7 @@
       <c r="K79" s="216"/>
     </row>
     <row r="80" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E80" s="211"/>
+      <c r="E80" s="208"/>
       <c r="F80" s="2" t="s">
         <v>58</v>
       </c>
@@ -9430,7 +9310,7 @@
       <c r="K80" s="217"/>
     </row>
     <row r="81" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E81" s="211"/>
+      <c r="E81" s="208"/>
       <c r="F81" s="2" t="s">
         <v>59</v>
       </c>
@@ -9446,12 +9326,12 @@
       <c r="J81" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K81" s="207" t="s">
+      <c r="K81" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E82" s="211"/>
+      <c r="E82" s="208"/>
       <c r="F82" s="2" t="s">
         <v>60</v>
       </c>
@@ -9467,10 +9347,10 @@
       <c r="J82" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K82" s="208"/>
+      <c r="K82" s="211"/>
     </row>
     <row r="83" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E83" s="211"/>
+      <c r="E83" s="208"/>
       <c r="F83" s="2" t="s">
         <v>61</v>
       </c>
@@ -9486,10 +9366,10 @@
       <c r="J83" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K83" s="208"/>
+      <c r="K83" s="211"/>
     </row>
     <row r="84" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E84" s="211"/>
+      <c r="E84" s="208"/>
       <c r="F84" s="2" t="s">
         <v>62</v>
       </c>
@@ -9505,10 +9385,10 @@
       <c r="J84" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K84" s="208"/>
+      <c r="K84" s="211"/>
     </row>
     <row r="85" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E85" s="211"/>
+      <c r="E85" s="208"/>
       <c r="F85" s="2" t="s">
         <v>63</v>
       </c>
@@ -9524,10 +9404,10 @@
       <c r="J85" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K85" s="208"/>
+      <c r="K85" s="211"/>
     </row>
     <row r="86" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E86" s="211"/>
+      <c r="E86" s="208"/>
       <c r="F86" s="2" t="s">
         <v>64</v>
       </c>
@@ -9543,10 +9423,10 @@
       <c r="J86" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K86" s="208"/>
+      <c r="K86" s="211"/>
     </row>
     <row r="87" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E87" s="211"/>
+      <c r="E87" s="208"/>
       <c r="F87" s="2" t="s">
         <v>65</v>
       </c>
@@ -9562,10 +9442,10 @@
       <c r="J87" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K87" s="208"/>
+      <c r="K87" s="211"/>
     </row>
     <row r="88" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E88" s="211"/>
+      <c r="E88" s="208"/>
       <c r="F88" s="2" t="s">
         <v>66</v>
       </c>
@@ -9581,10 +9461,10 @@
       <c r="J88" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K88" s="208"/>
+      <c r="K88" s="211"/>
     </row>
     <row r="89" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E89" s="211"/>
+      <c r="E89" s="208"/>
       <c r="F89" s="2" t="s">
         <v>67</v>
       </c>
@@ -9600,10 +9480,10 @@
       <c r="J89" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K89" s="208"/>
+      <c r="K89" s="211"/>
     </row>
     <row r="90" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E90" s="211"/>
+      <c r="E90" s="208"/>
       <c r="F90" s="2" t="s">
         <v>68</v>
       </c>
@@ -9619,10 +9499,10 @@
       <c r="J90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K90" s="208"/>
+      <c r="K90" s="211"/>
     </row>
     <row r="91" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E91" s="211"/>
+      <c r="E91" s="208"/>
       <c r="F91" s="2" t="s">
         <v>69</v>
       </c>
@@ -9638,10 +9518,10 @@
       <c r="J91" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K91" s="208"/>
+      <c r="K91" s="211"/>
     </row>
     <row r="92" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E92" s="211"/>
+      <c r="E92" s="208"/>
       <c r="F92" s="2" t="s">
         <v>70</v>
       </c>
@@ -9657,10 +9537,10 @@
       <c r="J92" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K92" s="208"/>
+      <c r="K92" s="211"/>
     </row>
     <row r="93" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E93" s="211"/>
+      <c r="E93" s="208"/>
       <c r="F93" s="2" t="s">
         <v>71</v>
       </c>
@@ -9676,10 +9556,10 @@
       <c r="J93" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K93" s="214"/>
+      <c r="K93" s="212"/>
     </row>
     <row r="94" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E94" s="211"/>
+      <c r="E94" s="208"/>
       <c r="F94" s="2" t="s">
         <v>72</v>
       </c>
@@ -9695,12 +9575,12 @@
       <c r="J94" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K94" s="207" t="s">
+      <c r="K94" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="95" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E95" s="211"/>
+      <c r="E95" s="208"/>
       <c r="F95" s="2" t="s">
         <v>73</v>
       </c>
@@ -9716,10 +9596,10 @@
       <c r="J95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K95" s="208"/>
+      <c r="K95" s="211"/>
     </row>
     <row r="96" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E96" s="212"/>
+      <c r="E96" s="209"/>
       <c r="F96" s="4" t="s">
         <v>74</v>
       </c>
@@ -9735,7 +9615,7 @@
       <c r="J96" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K96" s="209"/>
+      <c r="K96" s="214"/>
     </row>
     <row r="97" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F97" s="1"/>
@@ -9755,7 +9635,7 @@
     </row>
     <row r="98" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="99" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E99" s="210" t="s">
+      <c r="E99" s="207" t="s">
         <v>145</v>
       </c>
       <c r="F99" s="3" t="s">
@@ -9773,12 +9653,12 @@
       <c r="J99" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K99" s="213" t="s">
+      <c r="K99" s="210" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="100" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E100" s="211"/>
+      <c r="E100" s="208"/>
       <c r="F100" s="2" t="s">
         <v>57</v>
       </c>
@@ -9794,10 +9674,10 @@
       <c r="J100" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K100" s="208"/>
+      <c r="K100" s="211"/>
     </row>
     <row r="101" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E101" s="211"/>
+      <c r="E101" s="208"/>
       <c r="F101" s="2" t="s">
         <v>58</v>
       </c>
@@ -9813,10 +9693,10 @@
       <c r="J101" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="K101" s="214"/>
+      <c r="K101" s="212"/>
     </row>
     <row r="102" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E102" s="211"/>
+      <c r="E102" s="208"/>
       <c r="F102" s="2" t="s">
         <v>59</v>
       </c>
@@ -9832,12 +9712,12 @@
       <c r="J102" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K102" s="207" t="s">
+      <c r="K102" s="213" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="103" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E103" s="211"/>
+      <c r="E103" s="208"/>
       <c r="F103" s="2" t="s">
         <v>60</v>
       </c>
@@ -9853,10 +9733,10 @@
       <c r="J103" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K103" s="208"/>
+      <c r="K103" s="211"/>
     </row>
     <row r="104" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E104" s="211"/>
+      <c r="E104" s="208"/>
       <c r="F104" s="2" t="s">
         <v>61</v>
       </c>
@@ -9872,10 +9752,10 @@
       <c r="J104" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K104" s="208"/>
+      <c r="K104" s="211"/>
     </row>
     <row r="105" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E105" s="211"/>
+      <c r="E105" s="208"/>
       <c r="F105" s="2" t="s">
         <v>62</v>
       </c>
@@ -9891,10 +9771,10 @@
       <c r="J105" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K105" s="208"/>
+      <c r="K105" s="211"/>
     </row>
     <row r="106" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E106" s="211"/>
+      <c r="E106" s="208"/>
       <c r="F106" s="2" t="s">
         <v>63</v>
       </c>
@@ -9910,10 +9790,10 @@
       <c r="J106" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K106" s="208"/>
+      <c r="K106" s="211"/>
     </row>
     <row r="107" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E107" s="211"/>
+      <c r="E107" s="208"/>
       <c r="F107" s="2" t="s">
         <v>64</v>
       </c>
@@ -9929,10 +9809,10 @@
       <c r="J107" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K107" s="208"/>
+      <c r="K107" s="211"/>
     </row>
     <row r="108" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E108" s="211"/>
+      <c r="E108" s="208"/>
       <c r="F108" s="2" t="s">
         <v>65</v>
       </c>
@@ -9948,10 +9828,10 @@
       <c r="J108" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K108" s="208"/>
+      <c r="K108" s="211"/>
     </row>
     <row r="109" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E109" s="211"/>
+      <c r="E109" s="208"/>
       <c r="F109" s="2" t="s">
         <v>66</v>
       </c>
@@ -9967,10 +9847,10 @@
       <c r="J109" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K109" s="208"/>
+      <c r="K109" s="211"/>
     </row>
     <row r="110" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E110" s="211"/>
+      <c r="E110" s="208"/>
       <c r="F110" s="2" t="s">
         <v>67</v>
       </c>
@@ -9986,10 +9866,10 @@
       <c r="J110" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K110" s="208"/>
+      <c r="K110" s="211"/>
     </row>
     <row r="111" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E111" s="211"/>
+      <c r="E111" s="208"/>
       <c r="F111" s="2" t="s">
         <v>68</v>
       </c>
@@ -10005,10 +9885,10 @@
       <c r="J111" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K111" s="208"/>
+      <c r="K111" s="211"/>
     </row>
     <row r="112" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E112" s="211"/>
+      <c r="E112" s="208"/>
       <c r="F112" s="2" t="s">
         <v>69</v>
       </c>
@@ -10024,10 +9904,10 @@
       <c r="J112" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K112" s="208"/>
+      <c r="K112" s="211"/>
     </row>
     <row r="113" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E113" s="211"/>
+      <c r="E113" s="208"/>
       <c r="F113" s="2" t="s">
         <v>70</v>
       </c>
@@ -10043,10 +9923,10 @@
       <c r="J113" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K113" s="208"/>
+      <c r="K113" s="211"/>
     </row>
     <row r="114" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E114" s="211"/>
+      <c r="E114" s="208"/>
       <c r="F114" s="2" t="s">
         <v>71</v>
       </c>
@@ -10062,10 +9942,10 @@
       <c r="J114" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="K114" s="208"/>
+      <c r="K114" s="211"/>
     </row>
     <row r="115" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E115" s="211"/>
+      <c r="E115" s="208"/>
       <c r="F115" s="2" t="s">
         <v>72</v>
       </c>
@@ -10081,10 +9961,10 @@
       <c r="J115" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K115" s="214"/>
+      <c r="K115" s="212"/>
     </row>
     <row r="116" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E116" s="211"/>
+      <c r="E116" s="208"/>
       <c r="F116" s="2" t="s">
         <v>73</v>
       </c>
@@ -10100,12 +9980,12 @@
       <c r="J116" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K116" s="207" t="s">
+      <c r="K116" s="213" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" spans="5:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E117" s="212"/>
+      <c r="E117" s="209"/>
       <c r="F117" s="4" t="s">
         <v>74</v>
       </c>
@@ -10121,7 +10001,7 @@
       <c r="J117" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K117" s="209"/>
+      <c r="K117" s="214"/>
     </row>
     <row r="118" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F118" s="1"/>
@@ -10142,6 +10022,18 @@
   </sheetData>
   <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
+    <mergeCell ref="K33:K36"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="E8:E20"/>
+    <mergeCell ref="E23:E36"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="K17:K20"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K26:K32"/>
     <mergeCell ref="E99:E117"/>
     <mergeCell ref="K99:K101"/>
     <mergeCell ref="K102:K115"/>
@@ -10158,18 +10050,6 @@
     <mergeCell ref="E39:E54"/>
     <mergeCell ref="E57:E75"/>
     <mergeCell ref="E78:E96"/>
-    <mergeCell ref="K33:K36"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="E8:E20"/>
-    <mergeCell ref="E23:E36"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K16"/>
-    <mergeCell ref="K17:K20"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="K26:K32"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:K21">
     <cfRule type="expression" dxfId="63" priority="7">
@@ -13737,18 +13617,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14353,7 +14221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O58"/>
   <sheetViews>
@@ -15347,4 +15215,123 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="190" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="192"/>
+    </row>
+    <row r="3" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="232" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="233"/>
+      <c r="H3" s="233"/>
+      <c r="I3" s="233"/>
+      <c r="J3" s="233"/>
+      <c r="K3" s="234"/>
+    </row>
+    <row r="5" spans="2:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="6">
+        <f>SUM(C6:C8)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="6">
+        <f>'Principal - ABP'!L19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="6">
+        <f>C13*10</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="C8F4" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>